<commit_message>
Chỉnh sửa lại nội dung theo yêu câu
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cac khach hang khong phat sinh don hang/CRMFXXX4_Bao cao KH khong phat sinh don hang.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cac khach hang khong phat sinh don hang/CRMFXXX4_Bao cao KH khong phat sinh don hang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Coverpage" sheetId="20" r:id="rId1"/>
@@ -1550,7 +1550,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="224">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2233,9 +2233,6 @@
     <t>Click RadioBttn</t>
   </si>
   <si>
-    <t>thực thi @SQL0001 và @SQL0002 đổ nguồn cho combo</t>
-  </si>
-  <si>
     <t>Truyền tham số @DivisionID để gọi màn hình in báo cáo</t>
   </si>
   <si>
@@ -2254,6 +2251,97 @@
   <si>
     <t>Sử dụng màn hình này để:
 In báo cáo Khách hàng không phát sinh đơn hàng</t>
+  </si>
+  <si>
+    <t>DropdownChecklist</t>
+  </si>
+  <si>
+    <t>Checkbox1</t>
+  </si>
+  <si>
+    <t>Từ Khách hàng</t>
+  </si>
+  <si>
+    <t>FromAccountID</t>
+  </si>
+  <si>
+    <t>AccountID</t>
+  </si>
+  <si>
+    <t>Nếu được Check vào thì đổ Combobox</t>
+  </si>
+  <si>
+    <t>Đến Khách hàng</t>
+  </si>
+  <si>
+    <t>ToAccountID</t>
+  </si>
+  <si>
+    <t>Xem trước</t>
+  </si>
+  <si>
+    <t>BttnView</t>
+  </si>
+  <si>
+    <t>Truyền tham số @DivisionID để gọi load báo cáo xem trước khi In</t>
+  </si>
+  <si>
+    <t>Click vào Button Xem trước</t>
+  </si>
+  <si>
+    <t>Đổ nguồn combobox Khách hàng</t>
+  </si>
+  <si>
+    <t>@SQL0003</t>
+  </si>
+  <si>
+    <t>Select AccountID, AccountName
+ From CRMT10101
+Where DivisionID = @DivisionID
+Order By AccountID</t>
+  </si>
+  <si>
+    <t>Load màn hình Báo cáo để xem trước khi in</t>
+  </si>
+  <si>
+    <t>@SQL0004</t>
+  </si>
+  <si>
+    <t>@DivisionID @DivisionIDList  @FromDate @ToDate   @IsDate  
+@CheckBox1
+@FromAccountID @ToAccountID 
+@UserID
+@PageNumber
+@PageSize</t>
+  </si>
+  <si>
+    <t>Biến môi trường @@DivisionIDList  @@FromDate @@ToDate   @@IsDate 
+@@CheckBox1
+@@FromAccountID @@ToAccountID
+Biến môi trường
+@@PageNumber
+@@PageSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXEC CRMP10107(
+ @DivisionID       VARCHAR(50),  
+  @DivisionIDList    NVARCHAR(2000), 
+  @FromDate         DATETIME,
+  @ToDate           DATETIME,
+  @IsDate           TINYINT,
+@CheckBox1 TINYINT,
+@FromAccountID       Varchar(50),
+  @ToAccountID         Varchar(50,
+  @UserID  VARCHAR(50),
+@PageNumber INT,
+@PageSize INT)
+</t>
+  </si>
+  <si>
+    <t>thực thi @SQL0001, @SQL0002, @SQL0003 đổ nguồn cho combo</t>
+  </si>
+  <si>
+    <t>Click vào BttnView thực thi @SQL0004 Load màn hình view trước khi In</t>
   </si>
 </sst>
 </file>
@@ -2984,9 +3072,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3108,6 +3193,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3403,19 +3491,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28012</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2495550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3435,8 +3523,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1" y="781051"/>
-          <a:ext cx="9391086" cy="3171824"/>
+          <a:off x="0" y="762000"/>
+          <a:ext cx="10125075" cy="4800600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3796,454 +3884,454 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="116" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="116" customWidth="1"/>
-    <col min="3" max="5" width="8" style="116"/>
-    <col min="6" max="6" width="61.7109375" style="116" customWidth="1"/>
-    <col min="7" max="7" width="8" style="116"/>
-    <col min="8" max="8" width="8" style="116" customWidth="1"/>
-    <col min="9" max="256" width="8" style="116"/>
-    <col min="257" max="257" width="10.28515625" style="116" customWidth="1"/>
-    <col min="258" max="258" width="13.42578125" style="116" customWidth="1"/>
-    <col min="259" max="261" width="8" style="116"/>
-    <col min="262" max="262" width="61.7109375" style="116" customWidth="1"/>
-    <col min="263" max="263" width="8" style="116"/>
-    <col min="264" max="264" width="8" style="116" customWidth="1"/>
-    <col min="265" max="512" width="8" style="116"/>
-    <col min="513" max="513" width="10.28515625" style="116" customWidth="1"/>
-    <col min="514" max="514" width="13.42578125" style="116" customWidth="1"/>
-    <col min="515" max="517" width="8" style="116"/>
-    <col min="518" max="518" width="61.7109375" style="116" customWidth="1"/>
-    <col min="519" max="519" width="8" style="116"/>
-    <col min="520" max="520" width="8" style="116" customWidth="1"/>
-    <col min="521" max="768" width="8" style="116"/>
-    <col min="769" max="769" width="10.28515625" style="116" customWidth="1"/>
-    <col min="770" max="770" width="13.42578125" style="116" customWidth="1"/>
-    <col min="771" max="773" width="8" style="116"/>
-    <col min="774" max="774" width="61.7109375" style="116" customWidth="1"/>
-    <col min="775" max="775" width="8" style="116"/>
-    <col min="776" max="776" width="8" style="116" customWidth="1"/>
-    <col min="777" max="1024" width="8" style="116"/>
-    <col min="1025" max="1025" width="10.28515625" style="116" customWidth="1"/>
-    <col min="1026" max="1026" width="13.42578125" style="116" customWidth="1"/>
-    <col min="1027" max="1029" width="8" style="116"/>
-    <col min="1030" max="1030" width="61.7109375" style="116" customWidth="1"/>
-    <col min="1031" max="1031" width="8" style="116"/>
-    <col min="1032" max="1032" width="8" style="116" customWidth="1"/>
-    <col min="1033" max="1280" width="8" style="116"/>
-    <col min="1281" max="1281" width="10.28515625" style="116" customWidth="1"/>
-    <col min="1282" max="1282" width="13.42578125" style="116" customWidth="1"/>
-    <col min="1283" max="1285" width="8" style="116"/>
-    <col min="1286" max="1286" width="61.7109375" style="116" customWidth="1"/>
-    <col min="1287" max="1287" width="8" style="116"/>
-    <col min="1288" max="1288" width="8" style="116" customWidth="1"/>
-    <col min="1289" max="1536" width="8" style="116"/>
-    <col min="1537" max="1537" width="10.28515625" style="116" customWidth="1"/>
-    <col min="1538" max="1538" width="13.42578125" style="116" customWidth="1"/>
-    <col min="1539" max="1541" width="8" style="116"/>
-    <col min="1542" max="1542" width="61.7109375" style="116" customWidth="1"/>
-    <col min="1543" max="1543" width="8" style="116"/>
-    <col min="1544" max="1544" width="8" style="116" customWidth="1"/>
-    <col min="1545" max="1792" width="8" style="116"/>
-    <col min="1793" max="1793" width="10.28515625" style="116" customWidth="1"/>
-    <col min="1794" max="1794" width="13.42578125" style="116" customWidth="1"/>
-    <col min="1795" max="1797" width="8" style="116"/>
-    <col min="1798" max="1798" width="61.7109375" style="116" customWidth="1"/>
-    <col min="1799" max="1799" width="8" style="116"/>
-    <col min="1800" max="1800" width="8" style="116" customWidth="1"/>
-    <col min="1801" max="2048" width="8" style="116"/>
-    <col min="2049" max="2049" width="10.28515625" style="116" customWidth="1"/>
-    <col min="2050" max="2050" width="13.42578125" style="116" customWidth="1"/>
-    <col min="2051" max="2053" width="8" style="116"/>
-    <col min="2054" max="2054" width="61.7109375" style="116" customWidth="1"/>
-    <col min="2055" max="2055" width="8" style="116"/>
-    <col min="2056" max="2056" width="8" style="116" customWidth="1"/>
-    <col min="2057" max="2304" width="8" style="116"/>
-    <col min="2305" max="2305" width="10.28515625" style="116" customWidth="1"/>
-    <col min="2306" max="2306" width="13.42578125" style="116" customWidth="1"/>
-    <col min="2307" max="2309" width="8" style="116"/>
-    <col min="2310" max="2310" width="61.7109375" style="116" customWidth="1"/>
-    <col min="2311" max="2311" width="8" style="116"/>
-    <col min="2312" max="2312" width="8" style="116" customWidth="1"/>
-    <col min="2313" max="2560" width="8" style="116"/>
-    <col min="2561" max="2561" width="10.28515625" style="116" customWidth="1"/>
-    <col min="2562" max="2562" width="13.42578125" style="116" customWidth="1"/>
-    <col min="2563" max="2565" width="8" style="116"/>
-    <col min="2566" max="2566" width="61.7109375" style="116" customWidth="1"/>
-    <col min="2567" max="2567" width="8" style="116"/>
-    <col min="2568" max="2568" width="8" style="116" customWidth="1"/>
-    <col min="2569" max="2816" width="8" style="116"/>
-    <col min="2817" max="2817" width="10.28515625" style="116" customWidth="1"/>
-    <col min="2818" max="2818" width="13.42578125" style="116" customWidth="1"/>
-    <col min="2819" max="2821" width="8" style="116"/>
-    <col min="2822" max="2822" width="61.7109375" style="116" customWidth="1"/>
-    <col min="2823" max="2823" width="8" style="116"/>
-    <col min="2824" max="2824" width="8" style="116" customWidth="1"/>
-    <col min="2825" max="3072" width="8" style="116"/>
-    <col min="3073" max="3073" width="10.28515625" style="116" customWidth="1"/>
-    <col min="3074" max="3074" width="13.42578125" style="116" customWidth="1"/>
-    <col min="3075" max="3077" width="8" style="116"/>
-    <col min="3078" max="3078" width="61.7109375" style="116" customWidth="1"/>
-    <col min="3079" max="3079" width="8" style="116"/>
-    <col min="3080" max="3080" width="8" style="116" customWidth="1"/>
-    <col min="3081" max="3328" width="8" style="116"/>
-    <col min="3329" max="3329" width="10.28515625" style="116" customWidth="1"/>
-    <col min="3330" max="3330" width="13.42578125" style="116" customWidth="1"/>
-    <col min="3331" max="3333" width="8" style="116"/>
-    <col min="3334" max="3334" width="61.7109375" style="116" customWidth="1"/>
-    <col min="3335" max="3335" width="8" style="116"/>
-    <col min="3336" max="3336" width="8" style="116" customWidth="1"/>
-    <col min="3337" max="3584" width="8" style="116"/>
-    <col min="3585" max="3585" width="10.28515625" style="116" customWidth="1"/>
-    <col min="3586" max="3586" width="13.42578125" style="116" customWidth="1"/>
-    <col min="3587" max="3589" width="8" style="116"/>
-    <col min="3590" max="3590" width="61.7109375" style="116" customWidth="1"/>
-    <col min="3591" max="3591" width="8" style="116"/>
-    <col min="3592" max="3592" width="8" style="116" customWidth="1"/>
-    <col min="3593" max="3840" width="8" style="116"/>
-    <col min="3841" max="3841" width="10.28515625" style="116" customWidth="1"/>
-    <col min="3842" max="3842" width="13.42578125" style="116" customWidth="1"/>
-    <col min="3843" max="3845" width="8" style="116"/>
-    <col min="3846" max="3846" width="61.7109375" style="116" customWidth="1"/>
-    <col min="3847" max="3847" width="8" style="116"/>
-    <col min="3848" max="3848" width="8" style="116" customWidth="1"/>
-    <col min="3849" max="4096" width="8" style="116"/>
-    <col min="4097" max="4097" width="10.28515625" style="116" customWidth="1"/>
-    <col min="4098" max="4098" width="13.42578125" style="116" customWidth="1"/>
-    <col min="4099" max="4101" width="8" style="116"/>
-    <col min="4102" max="4102" width="61.7109375" style="116" customWidth="1"/>
-    <col min="4103" max="4103" width="8" style="116"/>
-    <col min="4104" max="4104" width="8" style="116" customWidth="1"/>
-    <col min="4105" max="4352" width="8" style="116"/>
-    <col min="4353" max="4353" width="10.28515625" style="116" customWidth="1"/>
-    <col min="4354" max="4354" width="13.42578125" style="116" customWidth="1"/>
-    <col min="4355" max="4357" width="8" style="116"/>
-    <col min="4358" max="4358" width="61.7109375" style="116" customWidth="1"/>
-    <col min="4359" max="4359" width="8" style="116"/>
-    <col min="4360" max="4360" width="8" style="116" customWidth="1"/>
-    <col min="4361" max="4608" width="8" style="116"/>
-    <col min="4609" max="4609" width="10.28515625" style="116" customWidth="1"/>
-    <col min="4610" max="4610" width="13.42578125" style="116" customWidth="1"/>
-    <col min="4611" max="4613" width="8" style="116"/>
-    <col min="4614" max="4614" width="61.7109375" style="116" customWidth="1"/>
-    <col min="4615" max="4615" width="8" style="116"/>
-    <col min="4616" max="4616" width="8" style="116" customWidth="1"/>
-    <col min="4617" max="4864" width="8" style="116"/>
-    <col min="4865" max="4865" width="10.28515625" style="116" customWidth="1"/>
-    <col min="4866" max="4866" width="13.42578125" style="116" customWidth="1"/>
-    <col min="4867" max="4869" width="8" style="116"/>
-    <col min="4870" max="4870" width="61.7109375" style="116" customWidth="1"/>
-    <col min="4871" max="4871" width="8" style="116"/>
-    <col min="4872" max="4872" width="8" style="116" customWidth="1"/>
-    <col min="4873" max="5120" width="8" style="116"/>
-    <col min="5121" max="5121" width="10.28515625" style="116" customWidth="1"/>
-    <col min="5122" max="5122" width="13.42578125" style="116" customWidth="1"/>
-    <col min="5123" max="5125" width="8" style="116"/>
-    <col min="5126" max="5126" width="61.7109375" style="116" customWidth="1"/>
-    <col min="5127" max="5127" width="8" style="116"/>
-    <col min="5128" max="5128" width="8" style="116" customWidth="1"/>
-    <col min="5129" max="5376" width="8" style="116"/>
-    <col min="5377" max="5377" width="10.28515625" style="116" customWidth="1"/>
-    <col min="5378" max="5378" width="13.42578125" style="116" customWidth="1"/>
-    <col min="5379" max="5381" width="8" style="116"/>
-    <col min="5382" max="5382" width="61.7109375" style="116" customWidth="1"/>
-    <col min="5383" max="5383" width="8" style="116"/>
-    <col min="5384" max="5384" width="8" style="116" customWidth="1"/>
-    <col min="5385" max="5632" width="8" style="116"/>
-    <col min="5633" max="5633" width="10.28515625" style="116" customWidth="1"/>
-    <col min="5634" max="5634" width="13.42578125" style="116" customWidth="1"/>
-    <col min="5635" max="5637" width="8" style="116"/>
-    <col min="5638" max="5638" width="61.7109375" style="116" customWidth="1"/>
-    <col min="5639" max="5639" width="8" style="116"/>
-    <col min="5640" max="5640" width="8" style="116" customWidth="1"/>
-    <col min="5641" max="5888" width="8" style="116"/>
-    <col min="5889" max="5889" width="10.28515625" style="116" customWidth="1"/>
-    <col min="5890" max="5890" width="13.42578125" style="116" customWidth="1"/>
-    <col min="5891" max="5893" width="8" style="116"/>
-    <col min="5894" max="5894" width="61.7109375" style="116" customWidth="1"/>
-    <col min="5895" max="5895" width="8" style="116"/>
-    <col min="5896" max="5896" width="8" style="116" customWidth="1"/>
-    <col min="5897" max="6144" width="8" style="116"/>
-    <col min="6145" max="6145" width="10.28515625" style="116" customWidth="1"/>
-    <col min="6146" max="6146" width="13.42578125" style="116" customWidth="1"/>
-    <col min="6147" max="6149" width="8" style="116"/>
-    <col min="6150" max="6150" width="61.7109375" style="116" customWidth="1"/>
-    <col min="6151" max="6151" width="8" style="116"/>
-    <col min="6152" max="6152" width="8" style="116" customWidth="1"/>
-    <col min="6153" max="6400" width="8" style="116"/>
-    <col min="6401" max="6401" width="10.28515625" style="116" customWidth="1"/>
-    <col min="6402" max="6402" width="13.42578125" style="116" customWidth="1"/>
-    <col min="6403" max="6405" width="8" style="116"/>
-    <col min="6406" max="6406" width="61.7109375" style="116" customWidth="1"/>
-    <col min="6407" max="6407" width="8" style="116"/>
-    <col min="6408" max="6408" width="8" style="116" customWidth="1"/>
-    <col min="6409" max="6656" width="8" style="116"/>
-    <col min="6657" max="6657" width="10.28515625" style="116" customWidth="1"/>
-    <col min="6658" max="6658" width="13.42578125" style="116" customWidth="1"/>
-    <col min="6659" max="6661" width="8" style="116"/>
-    <col min="6662" max="6662" width="61.7109375" style="116" customWidth="1"/>
-    <col min="6663" max="6663" width="8" style="116"/>
-    <col min="6664" max="6664" width="8" style="116" customWidth="1"/>
-    <col min="6665" max="6912" width="8" style="116"/>
-    <col min="6913" max="6913" width="10.28515625" style="116" customWidth="1"/>
-    <col min="6914" max="6914" width="13.42578125" style="116" customWidth="1"/>
-    <col min="6915" max="6917" width="8" style="116"/>
-    <col min="6918" max="6918" width="61.7109375" style="116" customWidth="1"/>
-    <col min="6919" max="6919" width="8" style="116"/>
-    <col min="6920" max="6920" width="8" style="116" customWidth="1"/>
-    <col min="6921" max="7168" width="8" style="116"/>
-    <col min="7169" max="7169" width="10.28515625" style="116" customWidth="1"/>
-    <col min="7170" max="7170" width="13.42578125" style="116" customWidth="1"/>
-    <col min="7171" max="7173" width="8" style="116"/>
-    <col min="7174" max="7174" width="61.7109375" style="116" customWidth="1"/>
-    <col min="7175" max="7175" width="8" style="116"/>
-    <col min="7176" max="7176" width="8" style="116" customWidth="1"/>
-    <col min="7177" max="7424" width="8" style="116"/>
-    <col min="7425" max="7425" width="10.28515625" style="116" customWidth="1"/>
-    <col min="7426" max="7426" width="13.42578125" style="116" customWidth="1"/>
-    <col min="7427" max="7429" width="8" style="116"/>
-    <col min="7430" max="7430" width="61.7109375" style="116" customWidth="1"/>
-    <col min="7431" max="7431" width="8" style="116"/>
-    <col min="7432" max="7432" width="8" style="116" customWidth="1"/>
-    <col min="7433" max="7680" width="8" style="116"/>
-    <col min="7681" max="7681" width="10.28515625" style="116" customWidth="1"/>
-    <col min="7682" max="7682" width="13.42578125" style="116" customWidth="1"/>
-    <col min="7683" max="7685" width="8" style="116"/>
-    <col min="7686" max="7686" width="61.7109375" style="116" customWidth="1"/>
-    <col min="7687" max="7687" width="8" style="116"/>
-    <col min="7688" max="7688" width="8" style="116" customWidth="1"/>
-    <col min="7689" max="7936" width="8" style="116"/>
-    <col min="7937" max="7937" width="10.28515625" style="116" customWidth="1"/>
-    <col min="7938" max="7938" width="13.42578125" style="116" customWidth="1"/>
-    <col min="7939" max="7941" width="8" style="116"/>
-    <col min="7942" max="7942" width="61.7109375" style="116" customWidth="1"/>
-    <col min="7943" max="7943" width="8" style="116"/>
-    <col min="7944" max="7944" width="8" style="116" customWidth="1"/>
-    <col min="7945" max="8192" width="8" style="116"/>
-    <col min="8193" max="8193" width="10.28515625" style="116" customWidth="1"/>
-    <col min="8194" max="8194" width="13.42578125" style="116" customWidth="1"/>
-    <col min="8195" max="8197" width="8" style="116"/>
-    <col min="8198" max="8198" width="61.7109375" style="116" customWidth="1"/>
-    <col min="8199" max="8199" width="8" style="116"/>
-    <col min="8200" max="8200" width="8" style="116" customWidth="1"/>
-    <col min="8201" max="8448" width="8" style="116"/>
-    <col min="8449" max="8449" width="10.28515625" style="116" customWidth="1"/>
-    <col min="8450" max="8450" width="13.42578125" style="116" customWidth="1"/>
-    <col min="8451" max="8453" width="8" style="116"/>
-    <col min="8454" max="8454" width="61.7109375" style="116" customWidth="1"/>
-    <col min="8455" max="8455" width="8" style="116"/>
-    <col min="8456" max="8456" width="8" style="116" customWidth="1"/>
-    <col min="8457" max="8704" width="8" style="116"/>
-    <col min="8705" max="8705" width="10.28515625" style="116" customWidth="1"/>
-    <col min="8706" max="8706" width="13.42578125" style="116" customWidth="1"/>
-    <col min="8707" max="8709" width="8" style="116"/>
-    <col min="8710" max="8710" width="61.7109375" style="116" customWidth="1"/>
-    <col min="8711" max="8711" width="8" style="116"/>
-    <col min="8712" max="8712" width="8" style="116" customWidth="1"/>
-    <col min="8713" max="8960" width="8" style="116"/>
-    <col min="8961" max="8961" width="10.28515625" style="116" customWidth="1"/>
-    <col min="8962" max="8962" width="13.42578125" style="116" customWidth="1"/>
-    <col min="8963" max="8965" width="8" style="116"/>
-    <col min="8966" max="8966" width="61.7109375" style="116" customWidth="1"/>
-    <col min="8967" max="8967" width="8" style="116"/>
-    <col min="8968" max="8968" width="8" style="116" customWidth="1"/>
-    <col min="8969" max="9216" width="8" style="116"/>
-    <col min="9217" max="9217" width="10.28515625" style="116" customWidth="1"/>
-    <col min="9218" max="9218" width="13.42578125" style="116" customWidth="1"/>
-    <col min="9219" max="9221" width="8" style="116"/>
-    <col min="9222" max="9222" width="61.7109375" style="116" customWidth="1"/>
-    <col min="9223" max="9223" width="8" style="116"/>
-    <col min="9224" max="9224" width="8" style="116" customWidth="1"/>
-    <col min="9225" max="9472" width="8" style="116"/>
-    <col min="9473" max="9473" width="10.28515625" style="116" customWidth="1"/>
-    <col min="9474" max="9474" width="13.42578125" style="116" customWidth="1"/>
-    <col min="9475" max="9477" width="8" style="116"/>
-    <col min="9478" max="9478" width="61.7109375" style="116" customWidth="1"/>
-    <col min="9479" max="9479" width="8" style="116"/>
-    <col min="9480" max="9480" width="8" style="116" customWidth="1"/>
-    <col min="9481" max="9728" width="8" style="116"/>
-    <col min="9729" max="9729" width="10.28515625" style="116" customWidth="1"/>
-    <col min="9730" max="9730" width="13.42578125" style="116" customWidth="1"/>
-    <col min="9731" max="9733" width="8" style="116"/>
-    <col min="9734" max="9734" width="61.7109375" style="116" customWidth="1"/>
-    <col min="9735" max="9735" width="8" style="116"/>
-    <col min="9736" max="9736" width="8" style="116" customWidth="1"/>
-    <col min="9737" max="9984" width="8" style="116"/>
-    <col min="9985" max="9985" width="10.28515625" style="116" customWidth="1"/>
-    <col min="9986" max="9986" width="13.42578125" style="116" customWidth="1"/>
-    <col min="9987" max="9989" width="8" style="116"/>
-    <col min="9990" max="9990" width="61.7109375" style="116" customWidth="1"/>
-    <col min="9991" max="9991" width="8" style="116"/>
-    <col min="9992" max="9992" width="8" style="116" customWidth="1"/>
-    <col min="9993" max="10240" width="8" style="116"/>
-    <col min="10241" max="10241" width="10.28515625" style="116" customWidth="1"/>
-    <col min="10242" max="10242" width="13.42578125" style="116" customWidth="1"/>
-    <col min="10243" max="10245" width="8" style="116"/>
-    <col min="10246" max="10246" width="61.7109375" style="116" customWidth="1"/>
-    <col min="10247" max="10247" width="8" style="116"/>
-    <col min="10248" max="10248" width="8" style="116" customWidth="1"/>
-    <col min="10249" max="10496" width="8" style="116"/>
-    <col min="10497" max="10497" width="10.28515625" style="116" customWidth="1"/>
-    <col min="10498" max="10498" width="13.42578125" style="116" customWidth="1"/>
-    <col min="10499" max="10501" width="8" style="116"/>
-    <col min="10502" max="10502" width="61.7109375" style="116" customWidth="1"/>
-    <col min="10503" max="10503" width="8" style="116"/>
-    <col min="10504" max="10504" width="8" style="116" customWidth="1"/>
-    <col min="10505" max="10752" width="8" style="116"/>
-    <col min="10753" max="10753" width="10.28515625" style="116" customWidth="1"/>
-    <col min="10754" max="10754" width="13.42578125" style="116" customWidth="1"/>
-    <col min="10755" max="10757" width="8" style="116"/>
-    <col min="10758" max="10758" width="61.7109375" style="116" customWidth="1"/>
-    <col min="10759" max="10759" width="8" style="116"/>
-    <col min="10760" max="10760" width="8" style="116" customWidth="1"/>
-    <col min="10761" max="11008" width="8" style="116"/>
-    <col min="11009" max="11009" width="10.28515625" style="116" customWidth="1"/>
-    <col min="11010" max="11010" width="13.42578125" style="116" customWidth="1"/>
-    <col min="11011" max="11013" width="8" style="116"/>
-    <col min="11014" max="11014" width="61.7109375" style="116" customWidth="1"/>
-    <col min="11015" max="11015" width="8" style="116"/>
-    <col min="11016" max="11016" width="8" style="116" customWidth="1"/>
-    <col min="11017" max="11264" width="8" style="116"/>
-    <col min="11265" max="11265" width="10.28515625" style="116" customWidth="1"/>
-    <col min="11266" max="11266" width="13.42578125" style="116" customWidth="1"/>
-    <col min="11267" max="11269" width="8" style="116"/>
-    <col min="11270" max="11270" width="61.7109375" style="116" customWidth="1"/>
-    <col min="11271" max="11271" width="8" style="116"/>
-    <col min="11272" max="11272" width="8" style="116" customWidth="1"/>
-    <col min="11273" max="11520" width="8" style="116"/>
-    <col min="11521" max="11521" width="10.28515625" style="116" customWidth="1"/>
-    <col min="11522" max="11522" width="13.42578125" style="116" customWidth="1"/>
-    <col min="11523" max="11525" width="8" style="116"/>
-    <col min="11526" max="11526" width="61.7109375" style="116" customWidth="1"/>
-    <col min="11527" max="11527" width="8" style="116"/>
-    <col min="11528" max="11528" width="8" style="116" customWidth="1"/>
-    <col min="11529" max="11776" width="8" style="116"/>
-    <col min="11777" max="11777" width="10.28515625" style="116" customWidth="1"/>
-    <col min="11778" max="11778" width="13.42578125" style="116" customWidth="1"/>
-    <col min="11779" max="11781" width="8" style="116"/>
-    <col min="11782" max="11782" width="61.7109375" style="116" customWidth="1"/>
-    <col min="11783" max="11783" width="8" style="116"/>
-    <col min="11784" max="11784" width="8" style="116" customWidth="1"/>
-    <col min="11785" max="12032" width="8" style="116"/>
-    <col min="12033" max="12033" width="10.28515625" style="116" customWidth="1"/>
-    <col min="12034" max="12034" width="13.42578125" style="116" customWidth="1"/>
-    <col min="12035" max="12037" width="8" style="116"/>
-    <col min="12038" max="12038" width="61.7109375" style="116" customWidth="1"/>
-    <col min="12039" max="12039" width="8" style="116"/>
-    <col min="12040" max="12040" width="8" style="116" customWidth="1"/>
-    <col min="12041" max="12288" width="8" style="116"/>
-    <col min="12289" max="12289" width="10.28515625" style="116" customWidth="1"/>
-    <col min="12290" max="12290" width="13.42578125" style="116" customWidth="1"/>
-    <col min="12291" max="12293" width="8" style="116"/>
-    <col min="12294" max="12294" width="61.7109375" style="116" customWidth="1"/>
-    <col min="12295" max="12295" width="8" style="116"/>
-    <col min="12296" max="12296" width="8" style="116" customWidth="1"/>
-    <col min="12297" max="12544" width="8" style="116"/>
-    <col min="12545" max="12545" width="10.28515625" style="116" customWidth="1"/>
-    <col min="12546" max="12546" width="13.42578125" style="116" customWidth="1"/>
-    <col min="12547" max="12549" width="8" style="116"/>
-    <col min="12550" max="12550" width="61.7109375" style="116" customWidth="1"/>
-    <col min="12551" max="12551" width="8" style="116"/>
-    <col min="12552" max="12552" width="8" style="116" customWidth="1"/>
-    <col min="12553" max="12800" width="8" style="116"/>
-    <col min="12801" max="12801" width="10.28515625" style="116" customWidth="1"/>
-    <col min="12802" max="12802" width="13.42578125" style="116" customWidth="1"/>
-    <col min="12803" max="12805" width="8" style="116"/>
-    <col min="12806" max="12806" width="61.7109375" style="116" customWidth="1"/>
-    <col min="12807" max="12807" width="8" style="116"/>
-    <col min="12808" max="12808" width="8" style="116" customWidth="1"/>
-    <col min="12809" max="13056" width="8" style="116"/>
-    <col min="13057" max="13057" width="10.28515625" style="116" customWidth="1"/>
-    <col min="13058" max="13058" width="13.42578125" style="116" customWidth="1"/>
-    <col min="13059" max="13061" width="8" style="116"/>
-    <col min="13062" max="13062" width="61.7109375" style="116" customWidth="1"/>
-    <col min="13063" max="13063" width="8" style="116"/>
-    <col min="13064" max="13064" width="8" style="116" customWidth="1"/>
-    <col min="13065" max="13312" width="8" style="116"/>
-    <col min="13313" max="13313" width="10.28515625" style="116" customWidth="1"/>
-    <col min="13314" max="13314" width="13.42578125" style="116" customWidth="1"/>
-    <col min="13315" max="13317" width="8" style="116"/>
-    <col min="13318" max="13318" width="61.7109375" style="116" customWidth="1"/>
-    <col min="13319" max="13319" width="8" style="116"/>
-    <col min="13320" max="13320" width="8" style="116" customWidth="1"/>
-    <col min="13321" max="13568" width="8" style="116"/>
-    <col min="13569" max="13569" width="10.28515625" style="116" customWidth="1"/>
-    <col min="13570" max="13570" width="13.42578125" style="116" customWidth="1"/>
-    <col min="13571" max="13573" width="8" style="116"/>
-    <col min="13574" max="13574" width="61.7109375" style="116" customWidth="1"/>
-    <col min="13575" max="13575" width="8" style="116"/>
-    <col min="13576" max="13576" width="8" style="116" customWidth="1"/>
-    <col min="13577" max="13824" width="8" style="116"/>
-    <col min="13825" max="13825" width="10.28515625" style="116" customWidth="1"/>
-    <col min="13826" max="13826" width="13.42578125" style="116" customWidth="1"/>
-    <col min="13827" max="13829" width="8" style="116"/>
-    <col min="13830" max="13830" width="61.7109375" style="116" customWidth="1"/>
-    <col min="13831" max="13831" width="8" style="116"/>
-    <col min="13832" max="13832" width="8" style="116" customWidth="1"/>
-    <col min="13833" max="14080" width="8" style="116"/>
-    <col min="14081" max="14081" width="10.28515625" style="116" customWidth="1"/>
-    <col min="14082" max="14082" width="13.42578125" style="116" customWidth="1"/>
-    <col min="14083" max="14085" width="8" style="116"/>
-    <col min="14086" max="14086" width="61.7109375" style="116" customWidth="1"/>
-    <col min="14087" max="14087" width="8" style="116"/>
-    <col min="14088" max="14088" width="8" style="116" customWidth="1"/>
-    <col min="14089" max="14336" width="8" style="116"/>
-    <col min="14337" max="14337" width="10.28515625" style="116" customWidth="1"/>
-    <col min="14338" max="14338" width="13.42578125" style="116" customWidth="1"/>
-    <col min="14339" max="14341" width="8" style="116"/>
-    <col min="14342" max="14342" width="61.7109375" style="116" customWidth="1"/>
-    <col min="14343" max="14343" width="8" style="116"/>
-    <col min="14344" max="14344" width="8" style="116" customWidth="1"/>
-    <col min="14345" max="14592" width="8" style="116"/>
-    <col min="14593" max="14593" width="10.28515625" style="116" customWidth="1"/>
-    <col min="14594" max="14594" width="13.42578125" style="116" customWidth="1"/>
-    <col min="14595" max="14597" width="8" style="116"/>
-    <col min="14598" max="14598" width="61.7109375" style="116" customWidth="1"/>
-    <col min="14599" max="14599" width="8" style="116"/>
-    <col min="14600" max="14600" width="8" style="116" customWidth="1"/>
-    <col min="14601" max="14848" width="8" style="116"/>
-    <col min="14849" max="14849" width="10.28515625" style="116" customWidth="1"/>
-    <col min="14850" max="14850" width="13.42578125" style="116" customWidth="1"/>
-    <col min="14851" max="14853" width="8" style="116"/>
-    <col min="14854" max="14854" width="61.7109375" style="116" customWidth="1"/>
-    <col min="14855" max="14855" width="8" style="116"/>
-    <col min="14856" max="14856" width="8" style="116" customWidth="1"/>
-    <col min="14857" max="15104" width="8" style="116"/>
-    <col min="15105" max="15105" width="10.28515625" style="116" customWidth="1"/>
-    <col min="15106" max="15106" width="13.42578125" style="116" customWidth="1"/>
-    <col min="15107" max="15109" width="8" style="116"/>
-    <col min="15110" max="15110" width="61.7109375" style="116" customWidth="1"/>
-    <col min="15111" max="15111" width="8" style="116"/>
-    <col min="15112" max="15112" width="8" style="116" customWidth="1"/>
-    <col min="15113" max="15360" width="8" style="116"/>
-    <col min="15361" max="15361" width="10.28515625" style="116" customWidth="1"/>
-    <col min="15362" max="15362" width="13.42578125" style="116" customWidth="1"/>
-    <col min="15363" max="15365" width="8" style="116"/>
-    <col min="15366" max="15366" width="61.7109375" style="116" customWidth="1"/>
-    <col min="15367" max="15367" width="8" style="116"/>
-    <col min="15368" max="15368" width="8" style="116" customWidth="1"/>
-    <col min="15369" max="15616" width="8" style="116"/>
-    <col min="15617" max="15617" width="10.28515625" style="116" customWidth="1"/>
-    <col min="15618" max="15618" width="13.42578125" style="116" customWidth="1"/>
-    <col min="15619" max="15621" width="8" style="116"/>
-    <col min="15622" max="15622" width="61.7109375" style="116" customWidth="1"/>
-    <col min="15623" max="15623" width="8" style="116"/>
-    <col min="15624" max="15624" width="8" style="116" customWidth="1"/>
-    <col min="15625" max="15872" width="8" style="116"/>
-    <col min="15873" max="15873" width="10.28515625" style="116" customWidth="1"/>
-    <col min="15874" max="15874" width="13.42578125" style="116" customWidth="1"/>
-    <col min="15875" max="15877" width="8" style="116"/>
-    <col min="15878" max="15878" width="61.7109375" style="116" customWidth="1"/>
-    <col min="15879" max="15879" width="8" style="116"/>
-    <col min="15880" max="15880" width="8" style="116" customWidth="1"/>
-    <col min="15881" max="16128" width="8" style="116"/>
-    <col min="16129" max="16129" width="10.28515625" style="116" customWidth="1"/>
-    <col min="16130" max="16130" width="13.42578125" style="116" customWidth="1"/>
-    <col min="16131" max="16133" width="8" style="116"/>
-    <col min="16134" max="16134" width="61.7109375" style="116" customWidth="1"/>
-    <col min="16135" max="16135" width="8" style="116"/>
-    <col min="16136" max="16136" width="8" style="116" customWidth="1"/>
-    <col min="16137" max="16384" width="8" style="116"/>
+    <col min="1" max="1" width="10.28515625" style="115" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="115" customWidth="1"/>
+    <col min="3" max="5" width="8" style="115"/>
+    <col min="6" max="6" width="61.7109375" style="115" customWidth="1"/>
+    <col min="7" max="7" width="8" style="115"/>
+    <col min="8" max="8" width="8" style="115" customWidth="1"/>
+    <col min="9" max="256" width="8" style="115"/>
+    <col min="257" max="257" width="10.28515625" style="115" customWidth="1"/>
+    <col min="258" max="258" width="13.42578125" style="115" customWidth="1"/>
+    <col min="259" max="261" width="8" style="115"/>
+    <col min="262" max="262" width="61.7109375" style="115" customWidth="1"/>
+    <col min="263" max="263" width="8" style="115"/>
+    <col min="264" max="264" width="8" style="115" customWidth="1"/>
+    <col min="265" max="512" width="8" style="115"/>
+    <col min="513" max="513" width="10.28515625" style="115" customWidth="1"/>
+    <col min="514" max="514" width="13.42578125" style="115" customWidth="1"/>
+    <col min="515" max="517" width="8" style="115"/>
+    <col min="518" max="518" width="61.7109375" style="115" customWidth="1"/>
+    <col min="519" max="519" width="8" style="115"/>
+    <col min="520" max="520" width="8" style="115" customWidth="1"/>
+    <col min="521" max="768" width="8" style="115"/>
+    <col min="769" max="769" width="10.28515625" style="115" customWidth="1"/>
+    <col min="770" max="770" width="13.42578125" style="115" customWidth="1"/>
+    <col min="771" max="773" width="8" style="115"/>
+    <col min="774" max="774" width="61.7109375" style="115" customWidth="1"/>
+    <col min="775" max="775" width="8" style="115"/>
+    <col min="776" max="776" width="8" style="115" customWidth="1"/>
+    <col min="777" max="1024" width="8" style="115"/>
+    <col min="1025" max="1025" width="10.28515625" style="115" customWidth="1"/>
+    <col min="1026" max="1026" width="13.42578125" style="115" customWidth="1"/>
+    <col min="1027" max="1029" width="8" style="115"/>
+    <col min="1030" max="1030" width="61.7109375" style="115" customWidth="1"/>
+    <col min="1031" max="1031" width="8" style="115"/>
+    <col min="1032" max="1032" width="8" style="115" customWidth="1"/>
+    <col min="1033" max="1280" width="8" style="115"/>
+    <col min="1281" max="1281" width="10.28515625" style="115" customWidth="1"/>
+    <col min="1282" max="1282" width="13.42578125" style="115" customWidth="1"/>
+    <col min="1283" max="1285" width="8" style="115"/>
+    <col min="1286" max="1286" width="61.7109375" style="115" customWidth="1"/>
+    <col min="1287" max="1287" width="8" style="115"/>
+    <col min="1288" max="1288" width="8" style="115" customWidth="1"/>
+    <col min="1289" max="1536" width="8" style="115"/>
+    <col min="1537" max="1537" width="10.28515625" style="115" customWidth="1"/>
+    <col min="1538" max="1538" width="13.42578125" style="115" customWidth="1"/>
+    <col min="1539" max="1541" width="8" style="115"/>
+    <col min="1542" max="1542" width="61.7109375" style="115" customWidth="1"/>
+    <col min="1543" max="1543" width="8" style="115"/>
+    <col min="1544" max="1544" width="8" style="115" customWidth="1"/>
+    <col min="1545" max="1792" width="8" style="115"/>
+    <col min="1793" max="1793" width="10.28515625" style="115" customWidth="1"/>
+    <col min="1794" max="1794" width="13.42578125" style="115" customWidth="1"/>
+    <col min="1795" max="1797" width="8" style="115"/>
+    <col min="1798" max="1798" width="61.7109375" style="115" customWidth="1"/>
+    <col min="1799" max="1799" width="8" style="115"/>
+    <col min="1800" max="1800" width="8" style="115" customWidth="1"/>
+    <col min="1801" max="2048" width="8" style="115"/>
+    <col min="2049" max="2049" width="10.28515625" style="115" customWidth="1"/>
+    <col min="2050" max="2050" width="13.42578125" style="115" customWidth="1"/>
+    <col min="2051" max="2053" width="8" style="115"/>
+    <col min="2054" max="2054" width="61.7109375" style="115" customWidth="1"/>
+    <col min="2055" max="2055" width="8" style="115"/>
+    <col min="2056" max="2056" width="8" style="115" customWidth="1"/>
+    <col min="2057" max="2304" width="8" style="115"/>
+    <col min="2305" max="2305" width="10.28515625" style="115" customWidth="1"/>
+    <col min="2306" max="2306" width="13.42578125" style="115" customWidth="1"/>
+    <col min="2307" max="2309" width="8" style="115"/>
+    <col min="2310" max="2310" width="61.7109375" style="115" customWidth="1"/>
+    <col min="2311" max="2311" width="8" style="115"/>
+    <col min="2312" max="2312" width="8" style="115" customWidth="1"/>
+    <col min="2313" max="2560" width="8" style="115"/>
+    <col min="2561" max="2561" width="10.28515625" style="115" customWidth="1"/>
+    <col min="2562" max="2562" width="13.42578125" style="115" customWidth="1"/>
+    <col min="2563" max="2565" width="8" style="115"/>
+    <col min="2566" max="2566" width="61.7109375" style="115" customWidth="1"/>
+    <col min="2567" max="2567" width="8" style="115"/>
+    <col min="2568" max="2568" width="8" style="115" customWidth="1"/>
+    <col min="2569" max="2816" width="8" style="115"/>
+    <col min="2817" max="2817" width="10.28515625" style="115" customWidth="1"/>
+    <col min="2818" max="2818" width="13.42578125" style="115" customWidth="1"/>
+    <col min="2819" max="2821" width="8" style="115"/>
+    <col min="2822" max="2822" width="61.7109375" style="115" customWidth="1"/>
+    <col min="2823" max="2823" width="8" style="115"/>
+    <col min="2824" max="2824" width="8" style="115" customWidth="1"/>
+    <col min="2825" max="3072" width="8" style="115"/>
+    <col min="3073" max="3073" width="10.28515625" style="115" customWidth="1"/>
+    <col min="3074" max="3074" width="13.42578125" style="115" customWidth="1"/>
+    <col min="3075" max="3077" width="8" style="115"/>
+    <col min="3078" max="3078" width="61.7109375" style="115" customWidth="1"/>
+    <col min="3079" max="3079" width="8" style="115"/>
+    <col min="3080" max="3080" width="8" style="115" customWidth="1"/>
+    <col min="3081" max="3328" width="8" style="115"/>
+    <col min="3329" max="3329" width="10.28515625" style="115" customWidth="1"/>
+    <col min="3330" max="3330" width="13.42578125" style="115" customWidth="1"/>
+    <col min="3331" max="3333" width="8" style="115"/>
+    <col min="3334" max="3334" width="61.7109375" style="115" customWidth="1"/>
+    <col min="3335" max="3335" width="8" style="115"/>
+    <col min="3336" max="3336" width="8" style="115" customWidth="1"/>
+    <col min="3337" max="3584" width="8" style="115"/>
+    <col min="3585" max="3585" width="10.28515625" style="115" customWidth="1"/>
+    <col min="3586" max="3586" width="13.42578125" style="115" customWidth="1"/>
+    <col min="3587" max="3589" width="8" style="115"/>
+    <col min="3590" max="3590" width="61.7109375" style="115" customWidth="1"/>
+    <col min="3591" max="3591" width="8" style="115"/>
+    <col min="3592" max="3592" width="8" style="115" customWidth="1"/>
+    <col min="3593" max="3840" width="8" style="115"/>
+    <col min="3841" max="3841" width="10.28515625" style="115" customWidth="1"/>
+    <col min="3842" max="3842" width="13.42578125" style="115" customWidth="1"/>
+    <col min="3843" max="3845" width="8" style="115"/>
+    <col min="3846" max="3846" width="61.7109375" style="115" customWidth="1"/>
+    <col min="3847" max="3847" width="8" style="115"/>
+    <col min="3848" max="3848" width="8" style="115" customWidth="1"/>
+    <col min="3849" max="4096" width="8" style="115"/>
+    <col min="4097" max="4097" width="10.28515625" style="115" customWidth="1"/>
+    <col min="4098" max="4098" width="13.42578125" style="115" customWidth="1"/>
+    <col min="4099" max="4101" width="8" style="115"/>
+    <col min="4102" max="4102" width="61.7109375" style="115" customWidth="1"/>
+    <col min="4103" max="4103" width="8" style="115"/>
+    <col min="4104" max="4104" width="8" style="115" customWidth="1"/>
+    <col min="4105" max="4352" width="8" style="115"/>
+    <col min="4353" max="4353" width="10.28515625" style="115" customWidth="1"/>
+    <col min="4354" max="4354" width="13.42578125" style="115" customWidth="1"/>
+    <col min="4355" max="4357" width="8" style="115"/>
+    <col min="4358" max="4358" width="61.7109375" style="115" customWidth="1"/>
+    <col min="4359" max="4359" width="8" style="115"/>
+    <col min="4360" max="4360" width="8" style="115" customWidth="1"/>
+    <col min="4361" max="4608" width="8" style="115"/>
+    <col min="4609" max="4609" width="10.28515625" style="115" customWidth="1"/>
+    <col min="4610" max="4610" width="13.42578125" style="115" customWidth="1"/>
+    <col min="4611" max="4613" width="8" style="115"/>
+    <col min="4614" max="4614" width="61.7109375" style="115" customWidth="1"/>
+    <col min="4615" max="4615" width="8" style="115"/>
+    <col min="4616" max="4616" width="8" style="115" customWidth="1"/>
+    <col min="4617" max="4864" width="8" style="115"/>
+    <col min="4865" max="4865" width="10.28515625" style="115" customWidth="1"/>
+    <col min="4866" max="4866" width="13.42578125" style="115" customWidth="1"/>
+    <col min="4867" max="4869" width="8" style="115"/>
+    <col min="4870" max="4870" width="61.7109375" style="115" customWidth="1"/>
+    <col min="4871" max="4871" width="8" style="115"/>
+    <col min="4872" max="4872" width="8" style="115" customWidth="1"/>
+    <col min="4873" max="5120" width="8" style="115"/>
+    <col min="5121" max="5121" width="10.28515625" style="115" customWidth="1"/>
+    <col min="5122" max="5122" width="13.42578125" style="115" customWidth="1"/>
+    <col min="5123" max="5125" width="8" style="115"/>
+    <col min="5126" max="5126" width="61.7109375" style="115" customWidth="1"/>
+    <col min="5127" max="5127" width="8" style="115"/>
+    <col min="5128" max="5128" width="8" style="115" customWidth="1"/>
+    <col min="5129" max="5376" width="8" style="115"/>
+    <col min="5377" max="5377" width="10.28515625" style="115" customWidth="1"/>
+    <col min="5378" max="5378" width="13.42578125" style="115" customWidth="1"/>
+    <col min="5379" max="5381" width="8" style="115"/>
+    <col min="5382" max="5382" width="61.7109375" style="115" customWidth="1"/>
+    <col min="5383" max="5383" width="8" style="115"/>
+    <col min="5384" max="5384" width="8" style="115" customWidth="1"/>
+    <col min="5385" max="5632" width="8" style="115"/>
+    <col min="5633" max="5633" width="10.28515625" style="115" customWidth="1"/>
+    <col min="5634" max="5634" width="13.42578125" style="115" customWidth="1"/>
+    <col min="5635" max="5637" width="8" style="115"/>
+    <col min="5638" max="5638" width="61.7109375" style="115" customWidth="1"/>
+    <col min="5639" max="5639" width="8" style="115"/>
+    <col min="5640" max="5640" width="8" style="115" customWidth="1"/>
+    <col min="5641" max="5888" width="8" style="115"/>
+    <col min="5889" max="5889" width="10.28515625" style="115" customWidth="1"/>
+    <col min="5890" max="5890" width="13.42578125" style="115" customWidth="1"/>
+    <col min="5891" max="5893" width="8" style="115"/>
+    <col min="5894" max="5894" width="61.7109375" style="115" customWidth="1"/>
+    <col min="5895" max="5895" width="8" style="115"/>
+    <col min="5896" max="5896" width="8" style="115" customWidth="1"/>
+    <col min="5897" max="6144" width="8" style="115"/>
+    <col min="6145" max="6145" width="10.28515625" style="115" customWidth="1"/>
+    <col min="6146" max="6146" width="13.42578125" style="115" customWidth="1"/>
+    <col min="6147" max="6149" width="8" style="115"/>
+    <col min="6150" max="6150" width="61.7109375" style="115" customWidth="1"/>
+    <col min="6151" max="6151" width="8" style="115"/>
+    <col min="6152" max="6152" width="8" style="115" customWidth="1"/>
+    <col min="6153" max="6400" width="8" style="115"/>
+    <col min="6401" max="6401" width="10.28515625" style="115" customWidth="1"/>
+    <col min="6402" max="6402" width="13.42578125" style="115" customWidth="1"/>
+    <col min="6403" max="6405" width="8" style="115"/>
+    <col min="6406" max="6406" width="61.7109375" style="115" customWidth="1"/>
+    <col min="6407" max="6407" width="8" style="115"/>
+    <col min="6408" max="6408" width="8" style="115" customWidth="1"/>
+    <col min="6409" max="6656" width="8" style="115"/>
+    <col min="6657" max="6657" width="10.28515625" style="115" customWidth="1"/>
+    <col min="6658" max="6658" width="13.42578125" style="115" customWidth="1"/>
+    <col min="6659" max="6661" width="8" style="115"/>
+    <col min="6662" max="6662" width="61.7109375" style="115" customWidth="1"/>
+    <col min="6663" max="6663" width="8" style="115"/>
+    <col min="6664" max="6664" width="8" style="115" customWidth="1"/>
+    <col min="6665" max="6912" width="8" style="115"/>
+    <col min="6913" max="6913" width="10.28515625" style="115" customWidth="1"/>
+    <col min="6914" max="6914" width="13.42578125" style="115" customWidth="1"/>
+    <col min="6915" max="6917" width="8" style="115"/>
+    <col min="6918" max="6918" width="61.7109375" style="115" customWidth="1"/>
+    <col min="6919" max="6919" width="8" style="115"/>
+    <col min="6920" max="6920" width="8" style="115" customWidth="1"/>
+    <col min="6921" max="7168" width="8" style="115"/>
+    <col min="7169" max="7169" width="10.28515625" style="115" customWidth="1"/>
+    <col min="7170" max="7170" width="13.42578125" style="115" customWidth="1"/>
+    <col min="7171" max="7173" width="8" style="115"/>
+    <col min="7174" max="7174" width="61.7109375" style="115" customWidth="1"/>
+    <col min="7175" max="7175" width="8" style="115"/>
+    <col min="7176" max="7176" width="8" style="115" customWidth="1"/>
+    <col min="7177" max="7424" width="8" style="115"/>
+    <col min="7425" max="7425" width="10.28515625" style="115" customWidth="1"/>
+    <col min="7426" max="7426" width="13.42578125" style="115" customWidth="1"/>
+    <col min="7427" max="7429" width="8" style="115"/>
+    <col min="7430" max="7430" width="61.7109375" style="115" customWidth="1"/>
+    <col min="7431" max="7431" width="8" style="115"/>
+    <col min="7432" max="7432" width="8" style="115" customWidth="1"/>
+    <col min="7433" max="7680" width="8" style="115"/>
+    <col min="7681" max="7681" width="10.28515625" style="115" customWidth="1"/>
+    <col min="7682" max="7682" width="13.42578125" style="115" customWidth="1"/>
+    <col min="7683" max="7685" width="8" style="115"/>
+    <col min="7686" max="7686" width="61.7109375" style="115" customWidth="1"/>
+    <col min="7687" max="7687" width="8" style="115"/>
+    <col min="7688" max="7688" width="8" style="115" customWidth="1"/>
+    <col min="7689" max="7936" width="8" style="115"/>
+    <col min="7937" max="7937" width="10.28515625" style="115" customWidth="1"/>
+    <col min="7938" max="7938" width="13.42578125" style="115" customWidth="1"/>
+    <col min="7939" max="7941" width="8" style="115"/>
+    <col min="7942" max="7942" width="61.7109375" style="115" customWidth="1"/>
+    <col min="7943" max="7943" width="8" style="115"/>
+    <col min="7944" max="7944" width="8" style="115" customWidth="1"/>
+    <col min="7945" max="8192" width="8" style="115"/>
+    <col min="8193" max="8193" width="10.28515625" style="115" customWidth="1"/>
+    <col min="8194" max="8194" width="13.42578125" style="115" customWidth="1"/>
+    <col min="8195" max="8197" width="8" style="115"/>
+    <col min="8198" max="8198" width="61.7109375" style="115" customWidth="1"/>
+    <col min="8199" max="8199" width="8" style="115"/>
+    <col min="8200" max="8200" width="8" style="115" customWidth="1"/>
+    <col min="8201" max="8448" width="8" style="115"/>
+    <col min="8449" max="8449" width="10.28515625" style="115" customWidth="1"/>
+    <col min="8450" max="8450" width="13.42578125" style="115" customWidth="1"/>
+    <col min="8451" max="8453" width="8" style="115"/>
+    <col min="8454" max="8454" width="61.7109375" style="115" customWidth="1"/>
+    <col min="8455" max="8455" width="8" style="115"/>
+    <col min="8456" max="8456" width="8" style="115" customWidth="1"/>
+    <col min="8457" max="8704" width="8" style="115"/>
+    <col min="8705" max="8705" width="10.28515625" style="115" customWidth="1"/>
+    <col min="8706" max="8706" width="13.42578125" style="115" customWidth="1"/>
+    <col min="8707" max="8709" width="8" style="115"/>
+    <col min="8710" max="8710" width="61.7109375" style="115" customWidth="1"/>
+    <col min="8711" max="8711" width="8" style="115"/>
+    <col min="8712" max="8712" width="8" style="115" customWidth="1"/>
+    <col min="8713" max="8960" width="8" style="115"/>
+    <col min="8961" max="8961" width="10.28515625" style="115" customWidth="1"/>
+    <col min="8962" max="8962" width="13.42578125" style="115" customWidth="1"/>
+    <col min="8963" max="8965" width="8" style="115"/>
+    <col min="8966" max="8966" width="61.7109375" style="115" customWidth="1"/>
+    <col min="8967" max="8967" width="8" style="115"/>
+    <col min="8968" max="8968" width="8" style="115" customWidth="1"/>
+    <col min="8969" max="9216" width="8" style="115"/>
+    <col min="9217" max="9217" width="10.28515625" style="115" customWidth="1"/>
+    <col min="9218" max="9218" width="13.42578125" style="115" customWidth="1"/>
+    <col min="9219" max="9221" width="8" style="115"/>
+    <col min="9222" max="9222" width="61.7109375" style="115" customWidth="1"/>
+    <col min="9223" max="9223" width="8" style="115"/>
+    <col min="9224" max="9224" width="8" style="115" customWidth="1"/>
+    <col min="9225" max="9472" width="8" style="115"/>
+    <col min="9473" max="9473" width="10.28515625" style="115" customWidth="1"/>
+    <col min="9474" max="9474" width="13.42578125" style="115" customWidth="1"/>
+    <col min="9475" max="9477" width="8" style="115"/>
+    <col min="9478" max="9478" width="61.7109375" style="115" customWidth="1"/>
+    <col min="9479" max="9479" width="8" style="115"/>
+    <col min="9480" max="9480" width="8" style="115" customWidth="1"/>
+    <col min="9481" max="9728" width="8" style="115"/>
+    <col min="9729" max="9729" width="10.28515625" style="115" customWidth="1"/>
+    <col min="9730" max="9730" width="13.42578125" style="115" customWidth="1"/>
+    <col min="9731" max="9733" width="8" style="115"/>
+    <col min="9734" max="9734" width="61.7109375" style="115" customWidth="1"/>
+    <col min="9735" max="9735" width="8" style="115"/>
+    <col min="9736" max="9736" width="8" style="115" customWidth="1"/>
+    <col min="9737" max="9984" width="8" style="115"/>
+    <col min="9985" max="9985" width="10.28515625" style="115" customWidth="1"/>
+    <col min="9986" max="9986" width="13.42578125" style="115" customWidth="1"/>
+    <col min="9987" max="9989" width="8" style="115"/>
+    <col min="9990" max="9990" width="61.7109375" style="115" customWidth="1"/>
+    <col min="9991" max="9991" width="8" style="115"/>
+    <col min="9992" max="9992" width="8" style="115" customWidth="1"/>
+    <col min="9993" max="10240" width="8" style="115"/>
+    <col min="10241" max="10241" width="10.28515625" style="115" customWidth="1"/>
+    <col min="10242" max="10242" width="13.42578125" style="115" customWidth="1"/>
+    <col min="10243" max="10245" width="8" style="115"/>
+    <col min="10246" max="10246" width="61.7109375" style="115" customWidth="1"/>
+    <col min="10247" max="10247" width="8" style="115"/>
+    <col min="10248" max="10248" width="8" style="115" customWidth="1"/>
+    <col min="10249" max="10496" width="8" style="115"/>
+    <col min="10497" max="10497" width="10.28515625" style="115" customWidth="1"/>
+    <col min="10498" max="10498" width="13.42578125" style="115" customWidth="1"/>
+    <col min="10499" max="10501" width="8" style="115"/>
+    <col min="10502" max="10502" width="61.7109375" style="115" customWidth="1"/>
+    <col min="10503" max="10503" width="8" style="115"/>
+    <col min="10504" max="10504" width="8" style="115" customWidth="1"/>
+    <col min="10505" max="10752" width="8" style="115"/>
+    <col min="10753" max="10753" width="10.28515625" style="115" customWidth="1"/>
+    <col min="10754" max="10754" width="13.42578125" style="115" customWidth="1"/>
+    <col min="10755" max="10757" width="8" style="115"/>
+    <col min="10758" max="10758" width="61.7109375" style="115" customWidth="1"/>
+    <col min="10759" max="10759" width="8" style="115"/>
+    <col min="10760" max="10760" width="8" style="115" customWidth="1"/>
+    <col min="10761" max="11008" width="8" style="115"/>
+    <col min="11009" max="11009" width="10.28515625" style="115" customWidth="1"/>
+    <col min="11010" max="11010" width="13.42578125" style="115" customWidth="1"/>
+    <col min="11011" max="11013" width="8" style="115"/>
+    <col min="11014" max="11014" width="61.7109375" style="115" customWidth="1"/>
+    <col min="11015" max="11015" width="8" style="115"/>
+    <col min="11016" max="11016" width="8" style="115" customWidth="1"/>
+    <col min="11017" max="11264" width="8" style="115"/>
+    <col min="11265" max="11265" width="10.28515625" style="115" customWidth="1"/>
+    <col min="11266" max="11266" width="13.42578125" style="115" customWidth="1"/>
+    <col min="11267" max="11269" width="8" style="115"/>
+    <col min="11270" max="11270" width="61.7109375" style="115" customWidth="1"/>
+    <col min="11271" max="11271" width="8" style="115"/>
+    <col min="11272" max="11272" width="8" style="115" customWidth="1"/>
+    <col min="11273" max="11520" width="8" style="115"/>
+    <col min="11521" max="11521" width="10.28515625" style="115" customWidth="1"/>
+    <col min="11522" max="11522" width="13.42578125" style="115" customWidth="1"/>
+    <col min="11523" max="11525" width="8" style="115"/>
+    <col min="11526" max="11526" width="61.7109375" style="115" customWidth="1"/>
+    <col min="11527" max="11527" width="8" style="115"/>
+    <col min="11528" max="11528" width="8" style="115" customWidth="1"/>
+    <col min="11529" max="11776" width="8" style="115"/>
+    <col min="11777" max="11777" width="10.28515625" style="115" customWidth="1"/>
+    <col min="11778" max="11778" width="13.42578125" style="115" customWidth="1"/>
+    <col min="11779" max="11781" width="8" style="115"/>
+    <col min="11782" max="11782" width="61.7109375" style="115" customWidth="1"/>
+    <col min="11783" max="11783" width="8" style="115"/>
+    <col min="11784" max="11784" width="8" style="115" customWidth="1"/>
+    <col min="11785" max="12032" width="8" style="115"/>
+    <col min="12033" max="12033" width="10.28515625" style="115" customWidth="1"/>
+    <col min="12034" max="12034" width="13.42578125" style="115" customWidth="1"/>
+    <col min="12035" max="12037" width="8" style="115"/>
+    <col min="12038" max="12038" width="61.7109375" style="115" customWidth="1"/>
+    <col min="12039" max="12039" width="8" style="115"/>
+    <col min="12040" max="12040" width="8" style="115" customWidth="1"/>
+    <col min="12041" max="12288" width="8" style="115"/>
+    <col min="12289" max="12289" width="10.28515625" style="115" customWidth="1"/>
+    <col min="12290" max="12290" width="13.42578125" style="115" customWidth="1"/>
+    <col min="12291" max="12293" width="8" style="115"/>
+    <col min="12294" max="12294" width="61.7109375" style="115" customWidth="1"/>
+    <col min="12295" max="12295" width="8" style="115"/>
+    <col min="12296" max="12296" width="8" style="115" customWidth="1"/>
+    <col min="12297" max="12544" width="8" style="115"/>
+    <col min="12545" max="12545" width="10.28515625" style="115" customWidth="1"/>
+    <col min="12546" max="12546" width="13.42578125" style="115" customWidth="1"/>
+    <col min="12547" max="12549" width="8" style="115"/>
+    <col min="12550" max="12550" width="61.7109375" style="115" customWidth="1"/>
+    <col min="12551" max="12551" width="8" style="115"/>
+    <col min="12552" max="12552" width="8" style="115" customWidth="1"/>
+    <col min="12553" max="12800" width="8" style="115"/>
+    <col min="12801" max="12801" width="10.28515625" style="115" customWidth="1"/>
+    <col min="12802" max="12802" width="13.42578125" style="115" customWidth="1"/>
+    <col min="12803" max="12805" width="8" style="115"/>
+    <col min="12806" max="12806" width="61.7109375" style="115" customWidth="1"/>
+    <col min="12807" max="12807" width="8" style="115"/>
+    <col min="12808" max="12808" width="8" style="115" customWidth="1"/>
+    <col min="12809" max="13056" width="8" style="115"/>
+    <col min="13057" max="13057" width="10.28515625" style="115" customWidth="1"/>
+    <col min="13058" max="13058" width="13.42578125" style="115" customWidth="1"/>
+    <col min="13059" max="13061" width="8" style="115"/>
+    <col min="13062" max="13062" width="61.7109375" style="115" customWidth="1"/>
+    <col min="13063" max="13063" width="8" style="115"/>
+    <col min="13064" max="13064" width="8" style="115" customWidth="1"/>
+    <col min="13065" max="13312" width="8" style="115"/>
+    <col min="13313" max="13313" width="10.28515625" style="115" customWidth="1"/>
+    <col min="13314" max="13314" width="13.42578125" style="115" customWidth="1"/>
+    <col min="13315" max="13317" width="8" style="115"/>
+    <col min="13318" max="13318" width="61.7109375" style="115" customWidth="1"/>
+    <col min="13319" max="13319" width="8" style="115"/>
+    <col min="13320" max="13320" width="8" style="115" customWidth="1"/>
+    <col min="13321" max="13568" width="8" style="115"/>
+    <col min="13569" max="13569" width="10.28515625" style="115" customWidth="1"/>
+    <col min="13570" max="13570" width="13.42578125" style="115" customWidth="1"/>
+    <col min="13571" max="13573" width="8" style="115"/>
+    <col min="13574" max="13574" width="61.7109375" style="115" customWidth="1"/>
+    <col min="13575" max="13575" width="8" style="115"/>
+    <col min="13576" max="13576" width="8" style="115" customWidth="1"/>
+    <col min="13577" max="13824" width="8" style="115"/>
+    <col min="13825" max="13825" width="10.28515625" style="115" customWidth="1"/>
+    <col min="13826" max="13826" width="13.42578125" style="115" customWidth="1"/>
+    <col min="13827" max="13829" width="8" style="115"/>
+    <col min="13830" max="13830" width="61.7109375" style="115" customWidth="1"/>
+    <col min="13831" max="13831" width="8" style="115"/>
+    <col min="13832" max="13832" width="8" style="115" customWidth="1"/>
+    <col min="13833" max="14080" width="8" style="115"/>
+    <col min="14081" max="14081" width="10.28515625" style="115" customWidth="1"/>
+    <col min="14082" max="14082" width="13.42578125" style="115" customWidth="1"/>
+    <col min="14083" max="14085" width="8" style="115"/>
+    <col min="14086" max="14086" width="61.7109375" style="115" customWidth="1"/>
+    <col min="14087" max="14087" width="8" style="115"/>
+    <col min="14088" max="14088" width="8" style="115" customWidth="1"/>
+    <col min="14089" max="14336" width="8" style="115"/>
+    <col min="14337" max="14337" width="10.28515625" style="115" customWidth="1"/>
+    <col min="14338" max="14338" width="13.42578125" style="115" customWidth="1"/>
+    <col min="14339" max="14341" width="8" style="115"/>
+    <col min="14342" max="14342" width="61.7109375" style="115" customWidth="1"/>
+    <col min="14343" max="14343" width="8" style="115"/>
+    <col min="14344" max="14344" width="8" style="115" customWidth="1"/>
+    <col min="14345" max="14592" width="8" style="115"/>
+    <col min="14593" max="14593" width="10.28515625" style="115" customWidth="1"/>
+    <col min="14594" max="14594" width="13.42578125" style="115" customWidth="1"/>
+    <col min="14595" max="14597" width="8" style="115"/>
+    <col min="14598" max="14598" width="61.7109375" style="115" customWidth="1"/>
+    <col min="14599" max="14599" width="8" style="115"/>
+    <col min="14600" max="14600" width="8" style="115" customWidth="1"/>
+    <col min="14601" max="14848" width="8" style="115"/>
+    <col min="14849" max="14849" width="10.28515625" style="115" customWidth="1"/>
+    <col min="14850" max="14850" width="13.42578125" style="115" customWidth="1"/>
+    <col min="14851" max="14853" width="8" style="115"/>
+    <col min="14854" max="14854" width="61.7109375" style="115" customWidth="1"/>
+    <col min="14855" max="14855" width="8" style="115"/>
+    <col min="14856" max="14856" width="8" style="115" customWidth="1"/>
+    <col min="14857" max="15104" width="8" style="115"/>
+    <col min="15105" max="15105" width="10.28515625" style="115" customWidth="1"/>
+    <col min="15106" max="15106" width="13.42578125" style="115" customWidth="1"/>
+    <col min="15107" max="15109" width="8" style="115"/>
+    <col min="15110" max="15110" width="61.7109375" style="115" customWidth="1"/>
+    <col min="15111" max="15111" width="8" style="115"/>
+    <col min="15112" max="15112" width="8" style="115" customWidth="1"/>
+    <col min="15113" max="15360" width="8" style="115"/>
+    <col min="15361" max="15361" width="10.28515625" style="115" customWidth="1"/>
+    <col min="15362" max="15362" width="13.42578125" style="115" customWidth="1"/>
+    <col min="15363" max="15365" width="8" style="115"/>
+    <col min="15366" max="15366" width="61.7109375" style="115" customWidth="1"/>
+    <col min="15367" max="15367" width="8" style="115"/>
+    <col min="15368" max="15368" width="8" style="115" customWidth="1"/>
+    <col min="15369" max="15616" width="8" style="115"/>
+    <col min="15617" max="15617" width="10.28515625" style="115" customWidth="1"/>
+    <col min="15618" max="15618" width="13.42578125" style="115" customWidth="1"/>
+    <col min="15619" max="15621" width="8" style="115"/>
+    <col min="15622" max="15622" width="61.7109375" style="115" customWidth="1"/>
+    <col min="15623" max="15623" width="8" style="115"/>
+    <col min="15624" max="15624" width="8" style="115" customWidth="1"/>
+    <col min="15625" max="15872" width="8" style="115"/>
+    <col min="15873" max="15873" width="10.28515625" style="115" customWidth="1"/>
+    <col min="15874" max="15874" width="13.42578125" style="115" customWidth="1"/>
+    <col min="15875" max="15877" width="8" style="115"/>
+    <col min="15878" max="15878" width="61.7109375" style="115" customWidth="1"/>
+    <col min="15879" max="15879" width="8" style="115"/>
+    <col min="15880" max="15880" width="8" style="115" customWidth="1"/>
+    <col min="15881" max="16128" width="8" style="115"/>
+    <col min="16129" max="16129" width="10.28515625" style="115" customWidth="1"/>
+    <col min="16130" max="16130" width="13.42578125" style="115" customWidth="1"/>
+    <col min="16131" max="16133" width="8" style="115"/>
+    <col min="16134" max="16134" width="61.7109375" style="115" customWidth="1"/>
+    <col min="16135" max="16135" width="8" style="115"/>
+    <col min="16136" max="16136" width="8" style="115" customWidth="1"/>
+    <col min="16137" max="16384" width="8" style="115"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
@@ -4293,7 +4381,7 @@
       <c r="J3" s="142"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="H4" s="117"/>
+      <c r="H4" s="116"/>
     </row>
     <row r="13" spans="1:18" ht="30">
       <c r="A13" s="143"/>
@@ -4306,14 +4394,14 @@
       <c r="H13" s="143"/>
       <c r="I13" s="143"/>
       <c r="J13" s="143"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="118"/>
-      <c r="M13" s="118"/>
-      <c r="N13" s="118"/>
-      <c r="O13" s="118"/>
-      <c r="P13" s="118"/>
-      <c r="Q13" s="118"/>
-      <c r="R13" s="118"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="117"/>
+      <c r="O13" s="117"/>
+      <c r="P13" s="117"/>
+      <c r="Q13" s="117"/>
+      <c r="R13" s="117"/>
     </row>
     <row r="14" spans="1:18" ht="26.25">
       <c r="B14" s="137"/>
@@ -4366,14 +4454,14 @@
       <c r="H16" s="140"/>
       <c r="I16" s="140"/>
       <c r="J16" s="140"/>
-      <c r="K16" s="119"/>
-      <c r="L16" s="119"/>
-      <c r="M16" s="119"/>
-      <c r="N16" s="119"/>
-      <c r="O16" s="119"/>
-      <c r="P16" s="119"/>
-      <c r="Q16" s="119"/>
-      <c r="R16" s="119"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
+      <c r="P16" s="118"/>
+      <c r="Q16" s="118"/>
+      <c r="R16" s="118"/>
     </row>
     <row r="17" spans="1:195" ht="14.1" customHeight="1">
       <c r="B17" s="137"/>
@@ -4722,7 +4810,7 @@
       <c r="GJ28" s="134"/>
       <c r="GK28" s="134"/>
       <c r="GL28" s="134"/>
-      <c r="GM28" s="120"/>
+      <c r="GM28" s="119"/>
     </row>
     <row r="29" spans="1:195" ht="18">
       <c r="B29" s="135"/>
@@ -4754,14 +4842,14 @@
       <c r="H30" s="133"/>
       <c r="I30" s="133"/>
       <c r="J30" s="133"/>
-      <c r="K30" s="121"/>
-      <c r="L30" s="121"/>
-      <c r="M30" s="121"/>
-      <c r="N30" s="121"/>
-      <c r="O30" s="121"/>
-      <c r="P30" s="121"/>
-      <c r="Q30" s="121"/>
-      <c r="R30" s="121"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="120"/>
+      <c r="M30" s="120"/>
+      <c r="N30" s="120"/>
+      <c r="O30" s="120"/>
+      <c r="P30" s="120"/>
+      <c r="Q30" s="120"/>
+      <c r="R30" s="120"/>
     </row>
     <row r="31" spans="1:195" ht="13.5" customHeight="1">
       <c r="A31" s="133"/>
@@ -4774,14 +4862,14 @@
       <c r="H31" s="133"/>
       <c r="I31" s="133"/>
       <c r="J31" s="133"/>
-      <c r="K31" s="121"/>
-      <c r="L31" s="121"/>
-      <c r="M31" s="121"/>
-      <c r="N31" s="121"/>
-      <c r="O31" s="121"/>
-      <c r="P31" s="121"/>
-      <c r="Q31" s="121"/>
-      <c r="R31" s="121"/>
+      <c r="K31" s="120"/>
+      <c r="L31" s="120"/>
+      <c r="M31" s="120"/>
+      <c r="N31" s="120"/>
+      <c r="O31" s="120"/>
+      <c r="P31" s="120"/>
+      <c r="Q31" s="120"/>
+      <c r="R31" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -5268,82 +5356,82 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="106" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="107" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="108" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="108" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="108" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="107" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="108" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="107" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="108" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="107" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="108" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="108" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="108" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="107" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="108" t="s">
         <v>149</v>
       </c>
     </row>
@@ -5388,12 +5476,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="H1" s="99" t="s">
         <v>160</v>
       </c>
       <c r="I1" s="31" t="s">
@@ -5416,7 +5504,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>6</v>
@@ -5454,20 +5542,20 @@
       <c r="J4" s="163"/>
     </row>
     <row r="5" spans="1:10" s="25" customFormat="1" ht="24" customHeight="1">
-      <c r="A5" s="128">
+      <c r="A5" s="127">
         <v>1</v>
       </c>
-      <c r="B5" s="129">
+      <c r="B5" s="128">
         <v>1</v>
       </c>
       <c r="C5" s="37">
         <v>42401</v>
       </c>
-      <c r="D5" s="130" t="s">
+      <c r="D5" s="129" t="s">
         <v>160</v>
       </c>
       <c r="E5" s="164" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F5" s="165"/>
       <c r="G5" s="165"/>
@@ -5476,7 +5564,7 @@
       <c r="J5" s="165"/>
     </row>
     <row r="6" spans="1:10" ht="12.75">
-      <c r="A6" s="91">
+      <c r="A6" s="90">
         <v>2</v>
       </c>
       <c r="B6" s="41">
@@ -5492,7 +5580,7 @@
       <c r="J6" s="168"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1">
-      <c r="A7" s="92">
+      <c r="A7" s="91">
         <v>3</v>
       </c>
       <c r="B7" s="41">
@@ -5508,7 +5596,7 @@
       <c r="J7" s="158"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
-      <c r="A8" s="93">
+      <c r="A8" s="92">
         <v>4</v>
       </c>
       <c r="B8" s="41">
@@ -5524,7 +5612,7 @@
       <c r="J8" s="161"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
-      <c r="A9" s="94">
+      <c r="A9" s="93">
         <v>5</v>
       </c>
       <c r="B9" s="41">
@@ -5540,7 +5628,7 @@
       <c r="J9" s="158"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
-      <c r="A10" s="95">
+      <c r="A10" s="94">
         <v>6</v>
       </c>
       <c r="B10" s="41">
@@ -5556,7 +5644,7 @@
       <c r="J10" s="158"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
-      <c r="A11" s="96">
+      <c r="A11" s="95">
         <v>7</v>
       </c>
       <c r="B11" s="41">
@@ -5572,7 +5660,7 @@
       <c r="J11" s="158"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
-      <c r="A12" s="97">
+      <c r="A12" s="96">
         <v>8</v>
       </c>
       <c r="B12" s="41">
@@ -5588,7 +5676,7 @@
       <c r="J12" s="158"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
-      <c r="A13" s="98">
+      <c r="A13" s="97">
         <v>9</v>
       </c>
       <c r="B13" s="41">
@@ -5604,7 +5692,7 @@
       <c r="J13" s="158"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
-      <c r="A14" s="99">
+      <c r="A14" s="98">
         <v>10</v>
       </c>
       <c r="B14" s="41">
@@ -5636,7 +5724,7 @@
       <c r="J15" s="155"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
-      <c r="A16" s="91">
+      <c r="A16" s="90">
         <v>12</v>
       </c>
       <c r="B16" s="41">
@@ -5652,7 +5740,7 @@
       <c r="J16" s="155"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
-      <c r="A17" s="92">
+      <c r="A17" s="91">
         <v>13</v>
       </c>
       <c r="B17" s="41">
@@ -5668,7 +5756,7 @@
       <c r="J17" s="155"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
-      <c r="A18" s="93">
+      <c r="A18" s="92">
         <v>14</v>
       </c>
       <c r="B18" s="41">
@@ -5684,7 +5772,7 @@
       <c r="J18" s="155"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
-      <c r="A19" s="94">
+      <c r="A19" s="93">
         <v>15</v>
       </c>
       <c r="B19" s="41">
@@ -5700,7 +5788,7 @@
       <c r="J19" s="155"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
-      <c r="A20" s="95">
+      <c r="A20" s="94">
         <v>16</v>
       </c>
       <c r="B20" s="41">
@@ -5716,7 +5804,7 @@
       <c r="J20" s="155"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
-      <c r="A21" s="96">
+      <c r="A21" s="95">
         <v>17</v>
       </c>
       <c r="B21" s="41">
@@ -5732,7 +5820,7 @@
       <c r="J21" s="155"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
-      <c r="A22" s="97">
+      <c r="A22" s="96">
         <v>18</v>
       </c>
       <c r="B22" s="41">
@@ -5748,7 +5836,7 @@
       <c r="J22" s="155"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
-      <c r="A23" s="98">
+      <c r="A23" s="97">
         <v>19</v>
       </c>
       <c r="B23" s="41">
@@ -5764,7 +5852,7 @@
       <c r="J23" s="155"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
-      <c r="A24" s="99">
+      <c r="A24" s="98">
         <v>20</v>
       </c>
       <c r="B24" s="41">
@@ -5812,7 +5900,7 @@
       <c r="J26" s="155"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
-      <c r="A27" s="91">
+      <c r="A27" s="90">
         <v>23</v>
       </c>
       <c r="B27" s="41">
@@ -5828,7 +5916,7 @@
       <c r="J27" s="155"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
-      <c r="A28" s="92">
+      <c r="A28" s="91">
         <v>24</v>
       </c>
       <c r="B28" s="41">
@@ -5844,7 +5932,7 @@
       <c r="J28" s="155"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
-      <c r="A29" s="93">
+      <c r="A29" s="92">
         <v>25</v>
       </c>
       <c r="B29" s="41">
@@ -5860,7 +5948,7 @@
       <c r="J29" s="155"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
-      <c r="A30" s="94">
+      <c r="A30" s="93">
         <v>26</v>
       </c>
       <c r="B30" s="41">
@@ -5876,7 +5964,7 @@
       <c r="J30" s="155"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
-      <c r="A31" s="95">
+      <c r="A31" s="94">
         <v>27</v>
       </c>
       <c r="B31" s="41">
@@ -5892,7 +5980,7 @@
       <c r="J31" s="155"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
-      <c r="A32" s="96">
+      <c r="A32" s="95">
         <v>28</v>
       </c>
       <c r="B32" s="41">
@@ -5908,7 +5996,7 @@
       <c r="J32" s="155"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
-      <c r="A33" s="97">
+      <c r="A33" s="96">
         <v>29</v>
       </c>
       <c r="B33" s="41">
@@ -5924,7 +6012,7 @@
       <c r="J33" s="155"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
-      <c r="A34" s="98">
+      <c r="A34" s="97">
         <v>30</v>
       </c>
       <c r="B34" s="41">
@@ -5940,7 +6028,7 @@
       <c r="J34" s="155"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
-      <c r="A35" s="99">
+      <c r="A35" s="98">
         <v>31</v>
       </c>
       <c r="B35" s="41">
@@ -5972,7 +6060,7 @@
       <c r="J36" s="155"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
-      <c r="A37" s="91">
+      <c r="A37" s="90">
         <v>33</v>
       </c>
       <c r="B37" s="41">
@@ -5988,7 +6076,7 @@
       <c r="J37" s="155"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
-      <c r="A38" s="92">
+      <c r="A38" s="91">
         <v>34</v>
       </c>
       <c r="B38" s="41">
@@ -6004,7 +6092,7 @@
       <c r="J38" s="155"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
-      <c r="A39" s="93">
+      <c r="A39" s="92">
         <v>35</v>
       </c>
       <c r="B39" s="41">
@@ -6020,7 +6108,7 @@
       <c r="J39" s="155"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
-      <c r="A40" s="94">
+      <c r="A40" s="93">
         <v>36</v>
       </c>
       <c r="B40" s="41">
@@ -6036,7 +6124,7 @@
       <c r="J40" s="155"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
-      <c r="A41" s="95">
+      <c r="A41" s="94">
         <v>37</v>
       </c>
       <c r="B41" s="41">
@@ -6052,7 +6140,7 @@
       <c r="J41" s="155"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
-      <c r="A42" s="96">
+      <c r="A42" s="95">
         <v>38</v>
       </c>
       <c r="B42" s="41">
@@ -6146,7 +6234,7 @@
     <col min="5" max="5" width="12.85546875" style="22" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" style="22" customWidth="1"/>
     <col min="7" max="7" width="24" style="22" customWidth="1"/>
-    <col min="8" max="8" width="26" style="22" customWidth="1"/>
+    <col min="8" max="8" width="40.85546875" style="22" customWidth="1"/>
     <col min="9" max="9" width="12" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="22" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="22"/>
@@ -6242,7 +6330,7 @@
       <c r="G5" s="43"/>
       <c r="H5" s="44"/>
       <c r="I5" s="178" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J5" s="179"/>
     </row>
@@ -6736,7 +6824,7 @@
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6:I7"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -6778,7 +6866,7 @@
       </c>
       <c r="H1" s="185"/>
       <c r="I1" s="186" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J1" s="187"/>
       <c r="K1" s="188"/>
@@ -6890,7 +6978,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="83" t="str">
         <f>'Update History'!F1</f>
@@ -6954,7 +7042,7 @@
       <c r="E7" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="F7" s="127" t="s">
+      <c r="F7" s="126" t="s">
         <v>172</v>
       </c>
       <c r="G7" s="40" t="s">
@@ -6989,7 +7077,7 @@
       <c r="E8" s="88" t="s">
         <v>173</v>
       </c>
-      <c r="F8" s="127" t="s">
+      <c r="F8" s="126" t="s">
         <v>173</v>
       </c>
       <c r="G8" s="40" t="s">
@@ -7019,10 +7107,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="59"/>
-      <c r="E9" s="127" t="s">
+      <c r="E9" s="126" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="127"/>
+      <c r="F9" s="126"/>
       <c r="G9" s="40" t="s">
         <v>168</v>
       </c>
@@ -7050,27 +7138,27 @@
       <c r="D10" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="88" t="s">
+      <c r="E10" s="132" t="s">
         <v>175</v>
       </c>
-      <c r="F10" s="127" t="s">
+      <c r="F10" s="132" t="s">
         <v>175</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I10" s="62"/>
       <c r="J10" s="62"/>
       <c r="K10" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="88"/>
+      <c r="L10" s="132"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
     </row>
     <row r="11" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="33">
@@ -7085,14 +7173,14 @@
       <c r="D11" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="132" t="s">
         <v>176</v>
       </c>
-      <c r="F11" s="127" t="s">
+      <c r="F11" s="132" t="s">
         <v>176</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>178</v>
@@ -7102,10 +7190,10 @@
       </c>
       <c r="J11" s="62"/>
       <c r="K11" s="40"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="88"/>
+      <c r="L11" s="132"/>
+      <c r="M11" s="132"/>
+      <c r="N11" s="132"/>
+      <c r="O11" s="132"/>
     </row>
     <row r="12" spans="1:15" s="34" customFormat="1" ht="11.25">
       <c r="A12" s="33">
@@ -7117,100 +7205,156 @@
       <c r="C12" s="33">
         <v>8</v>
       </c>
-      <c r="D12" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="E12" s="88" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" s="88"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="132" t="s">
+        <v>203</v>
+      </c>
+      <c r="F12" s="132"/>
       <c r="G12" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H12" s="40"/>
       <c r="I12" s="62"/>
       <c r="J12" s="62"/>
       <c r="K12" s="40"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="88"/>
+      <c r="L12" s="132"/>
+      <c r="M12" s="132"/>
+      <c r="N12" s="132">
+        <v>0</v>
+      </c>
+      <c r="O12" s="132"/>
     </row>
     <row r="13" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
         <v>9</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="62"/>
+      <c r="B13" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="33">
+        <v>9</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="132" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="I13" s="62">
+        <v>50</v>
+      </c>
       <c r="J13" s="62"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="88"/>
+      <c r="K13" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="L13" s="132"/>
+      <c r="M13" s="132"/>
+      <c r="N13" s="132"/>
+      <c r="O13" s="132" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="14" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
         <v>10</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="62"/>
+      <c r="B14" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="33">
+        <v>10</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="132" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="132" t="s">
+        <v>206</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="I14" s="62">
+        <v>50</v>
+      </c>
       <c r="J14" s="62"/>
       <c r="K14" s="40"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="88"/>
+      <c r="L14" s="132"/>
+      <c r="M14" s="132"/>
+      <c r="N14" s="132"/>
+      <c r="O14" s="132"/>
     </row>
     <row r="15" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
         <v>11</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="40"/>
+      <c r="B15" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="33">
+        <v>11</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="132" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" s="132"/>
+      <c r="G15" s="40" t="s">
+        <v>169</v>
+      </c>
       <c r="H15" s="40"/>
       <c r="I15" s="62"/>
       <c r="J15" s="62"/>
       <c r="K15" s="40"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="88"/>
+      <c r="L15" s="132"/>
+      <c r="M15" s="132"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="132"/>
     </row>
     <row r="16" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="33">
         <v>12</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="40"/>
+      <c r="B16" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="33">
+        <v>12</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" s="132"/>
+      <c r="G16" s="40" t="s">
+        <v>169</v>
+      </c>
       <c r="H16" s="40"/>
       <c r="I16" s="62"/>
       <c r="J16" s="62"/>
       <c r="K16" s="40"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="88"/>
+      <c r="L16" s="132"/>
+      <c r="M16" s="132"/>
+      <c r="N16" s="132"/>
+      <c r="O16" s="132"/>
     </row>
     <row r="17" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A17" s="33">
@@ -7219,17 +7363,17 @@
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
       <c r="D17" s="59"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
       <c r="G17" s="40"/>
       <c r="H17" s="40"/>
       <c r="I17" s="62"/>
-      <c r="J17" s="40"/>
+      <c r="J17" s="62"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="88"/>
+      <c r="L17" s="132"/>
+      <c r="M17" s="132"/>
+      <c r="N17" s="132"/>
+      <c r="O17" s="132"/>
     </row>
     <row r="18" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
@@ -7238,17 +7382,17 @@
       <c r="B18" s="33"/>
       <c r="C18" s="33"/>
       <c r="D18" s="59"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="132"/>
       <c r="G18" s="40"/>
       <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="88"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="132"/>
+      <c r="N18" s="132"/>
+      <c r="O18" s="132"/>
     </row>
     <row r="19" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
@@ -7942,7 +8086,7 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="I2:K2"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M25:N54 L24:M24">
       <formula1>"   ,l"</formula1>
     </dataValidation>
@@ -7953,8 +8097,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K54">
       <formula1>"I,O,I/O"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G9 G15:G54">
       <formula1>"Caption,Textbox,DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G12:G14">
+      <formula1>"Caption,Textbox,DropDownCheckList, DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G11">
+      <formula1>"Caption,Textbox,DropdownChecklist,DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7967,7 +8117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
@@ -7997,25 +8147,25 @@
         <v>1</v>
       </c>
       <c r="B1" s="30"/>
-      <c r="C1" s="105" t="str">
+      <c r="C1" s="104" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="105" t="str">
+      <c r="E1" s="104" t="str">
         <f>'Update History'!F1</f>
         <v>CRMFXXX4</v>
       </c>
       <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="112" t="str">
+      <c r="G1" s="111" t="str">
         <f>'Update History'!H1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="H1" s="104" t="s">
+      <c r="H1" s="103" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="67" t="s">
@@ -8028,14 +8178,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="30"/>
-      <c r="C2" s="105" t="str">
+      <c r="C2" s="104" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - CRM</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="105" t="str">
+      <c r="E2" s="104" t="str">
         <f>'Update History'!F2</f>
         <v>Báo cáo khách hàng không phát sinh đơn hàng</v>
       </c>
@@ -8046,7 +8196,7 @@
         <f>'Update History'!H2</f>
         <v>42401</v>
       </c>
-      <c r="H2" s="104" t="s">
+      <c r="H2" s="103" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="67">
@@ -8097,11 +8247,11 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="88"/>
-      <c r="D5" s="114"/>
+      <c r="D5" s="113"/>
       <c r="E5" s="40"/>
       <c r="F5" s="62"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="115"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
       <c r="I5" s="63"/>
       <c r="J5" s="69"/>
     </row>
@@ -8111,11 +8261,11 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="88"/>
-      <c r="D6" s="114"/>
+      <c r="D6" s="113"/>
       <c r="E6" s="40"/>
       <c r="F6" s="62"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
       <c r="I6" s="63"/>
       <c r="J6" s="69"/>
     </row>
@@ -8125,11 +8275,11 @@
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="88"/>
-      <c r="D7" s="114"/>
+      <c r="D7" s="113"/>
       <c r="E7" s="40"/>
       <c r="F7" s="62"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
       <c r="I7" s="63"/>
       <c r="J7" s="88"/>
     </row>
@@ -8139,11 +8289,11 @@
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="88"/>
-      <c r="D8" s="114"/>
+      <c r="D8" s="113"/>
       <c r="E8" s="40"/>
       <c r="F8" s="62"/>
-      <c r="G8" s="115"/>
-      <c r="H8" s="115"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
       <c r="I8" s="63"/>
       <c r="J8" s="88"/>
     </row>
@@ -8153,11 +8303,11 @@
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="88"/>
-      <c r="D9" s="114"/>
+      <c r="D9" s="113"/>
       <c r="E9" s="40"/>
       <c r="F9" s="62"/>
       <c r="G9" s="88"/>
-      <c r="H9" s="115"/>
+      <c r="H9" s="114"/>
       <c r="I9" s="63"/>
       <c r="J9" s="84"/>
     </row>
@@ -8202,7 +8352,7 @@
       <c r="H12" s="84"/>
       <c r="I12" s="82"/>
       <c r="J12" s="69"/>
-      <c r="K12" s="110"/>
+      <c r="K12" s="109"/>
     </row>
     <row r="13" spans="1:16" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -8217,7 +8367,7 @@
       <c r="H13" s="84"/>
       <c r="I13" s="82"/>
       <c r="J13" s="69"/>
-      <c r="K13" s="110"/>
+      <c r="K13" s="109"/>
     </row>
     <row r="14" spans="1:16" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -8232,7 +8382,7 @@
       <c r="H14" s="84"/>
       <c r="I14" s="82"/>
       <c r="J14" s="69"/>
-      <c r="K14" s="110"/>
+      <c r="K14" s="109"/>
     </row>
     <row r="15" spans="1:16" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
@@ -8247,7 +8397,7 @@
       <c r="H15" s="84"/>
       <c r="I15" s="82"/>
       <c r="J15" s="69"/>
-      <c r="K15" s="110"/>
+      <c r="K15" s="109"/>
     </row>
     <row r="16" spans="1:16" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="33">
@@ -8262,7 +8412,7 @@
       <c r="H16" s="69"/>
       <c r="I16" s="69"/>
       <c r="J16" s="69"/>
-      <c r="K16" s="110"/>
+      <c r="K16" s="109"/>
     </row>
     <row r="17" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A17" s="33">
@@ -8277,7 +8427,7 @@
       <c r="H17" s="69"/>
       <c r="I17" s="69"/>
       <c r="J17" s="69"/>
-      <c r="K17" s="110"/>
+      <c r="K17" s="109"/>
     </row>
     <row r="18" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
@@ -8292,7 +8442,7 @@
       <c r="H18" s="69"/>
       <c r="I18" s="69"/>
       <c r="J18" s="69"/>
-      <c r="K18" s="110"/>
+      <c r="K18" s="109"/>
     </row>
     <row r="19" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
@@ -8307,7 +8457,7 @@
       <c r="H19" s="69"/>
       <c r="I19" s="69"/>
       <c r="J19" s="69"/>
-      <c r="K19" s="110"/>
+      <c r="K19" s="109"/>
     </row>
     <row r="20" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="33">
@@ -8322,7 +8472,7 @@
       <c r="H20" s="69"/>
       <c r="I20" s="69"/>
       <c r="J20" s="69"/>
-      <c r="K20" s="110"/>
+      <c r="K20" s="109"/>
     </row>
     <row r="21" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="33">
@@ -8337,7 +8487,7 @@
       <c r="H21" s="69"/>
       <c r="I21" s="69"/>
       <c r="J21" s="69"/>
-      <c r="K21" s="110"/>
+      <c r="K21" s="109"/>
     </row>
     <row r="22" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="33">
@@ -8352,7 +8502,7 @@
       <c r="H22" s="69"/>
       <c r="I22" s="69"/>
       <c r="J22" s="69"/>
-      <c r="K22" s="110"/>
+      <c r="K22" s="109"/>
     </row>
     <row r="23" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="33">
@@ -8367,7 +8517,7 @@
       <c r="H23" s="69"/>
       <c r="I23" s="69"/>
       <c r="J23" s="69"/>
-      <c r="K23" s="110"/>
+      <c r="K23" s="109"/>
     </row>
     <row r="24" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="33">
@@ -8382,7 +8532,7 @@
       <c r="H24" s="69"/>
       <c r="I24" s="69"/>
       <c r="J24" s="69"/>
-      <c r="K24" s="110"/>
+      <c r="K24" s="109"/>
     </row>
     <row r="25" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="33">
@@ -8397,7 +8547,7 @@
       <c r="H25" s="69"/>
       <c r="I25" s="69"/>
       <c r="J25" s="69"/>
-      <c r="K25" s="110"/>
+      <c r="K25" s="109"/>
     </row>
     <row r="26" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="33">
@@ -8412,7 +8562,7 @@
       <c r="H26" s="62"/>
       <c r="I26" s="61"/>
       <c r="J26" s="62"/>
-      <c r="K26" s="111"/>
+      <c r="K26" s="110"/>
     </row>
     <row r="27" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="33">
@@ -8427,7 +8577,7 @@
       <c r="H27" s="62"/>
       <c r="I27" s="61"/>
       <c r="J27" s="62"/>
-      <c r="K27" s="111"/>
+      <c r="K27" s="110"/>
     </row>
     <row r="28" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="33">
@@ -8442,7 +8592,7 @@
       <c r="H28" s="62"/>
       <c r="I28" s="61"/>
       <c r="J28" s="62"/>
-      <c r="K28" s="111"/>
+      <c r="K28" s="110"/>
     </row>
     <row r="29" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33">
@@ -8457,7 +8607,7 @@
       <c r="H29" s="62"/>
       <c r="I29" s="61"/>
       <c r="J29" s="62"/>
-      <c r="K29" s="111"/>
+      <c r="K29" s="110"/>
     </row>
     <row r="30" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A30" s="33">
@@ -8472,7 +8622,7 @@
       <c r="H30" s="62"/>
       <c r="I30" s="61"/>
       <c r="J30" s="62"/>
-      <c r="K30" s="111"/>
+      <c r="K30" s="110"/>
     </row>
     <row r="31" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A31" s="33">
@@ -8487,7 +8637,7 @@
       <c r="H31" s="62"/>
       <c r="I31" s="61"/>
       <c r="J31" s="62"/>
-      <c r="K31" s="111"/>
+      <c r="K31" s="110"/>
     </row>
     <row r="32" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A32" s="33">
@@ -8502,7 +8652,7 @@
       <c r="H32" s="62"/>
       <c r="I32" s="61"/>
       <c r="J32" s="62"/>
-      <c r="K32" s="111"/>
+      <c r="K32" s="110"/>
     </row>
     <row r="33" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A33" s="33">
@@ -8517,7 +8667,7 @@
       <c r="H33" s="62"/>
       <c r="I33" s="61"/>
       <c r="J33" s="62"/>
-      <c r="K33" s="111"/>
+      <c r="K33" s="110"/>
     </row>
     <row r="34" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A34" s="33">
@@ -8532,7 +8682,7 @@
       <c r="H34" s="62"/>
       <c r="I34" s="61"/>
       <c r="J34" s="62"/>
-      <c r="K34" s="111"/>
+      <c r="K34" s="110"/>
     </row>
     <row r="35" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A35" s="33">
@@ -8547,7 +8697,7 @@
       <c r="H35" s="62"/>
       <c r="I35" s="61"/>
       <c r="J35" s="62"/>
-      <c r="K35" s="111"/>
+      <c r="K35" s="110"/>
     </row>
     <row r="36" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A36" s="33">
@@ -8562,7 +8712,7 @@
       <c r="H36" s="62"/>
       <c r="I36" s="61"/>
       <c r="J36" s="62"/>
-      <c r="K36" s="111"/>
+      <c r="K36" s="110"/>
     </row>
     <row r="37" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A37" s="33">
@@ -8577,7 +8727,7 @@
       <c r="H37" s="62"/>
       <c r="I37" s="61"/>
       <c r="J37" s="62"/>
-      <c r="K37" s="111"/>
+      <c r="K37" s="110"/>
     </row>
     <row r="38" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A38" s="33">
@@ -8592,7 +8742,7 @@
       <c r="H38" s="62"/>
       <c r="I38" s="61"/>
       <c r="J38" s="62"/>
-      <c r="K38" s="111"/>
+      <c r="K38" s="110"/>
     </row>
     <row r="39" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A39" s="33">
@@ -8607,7 +8757,7 @@
       <c r="H39" s="62"/>
       <c r="I39" s="61"/>
       <c r="J39" s="62"/>
-      <c r="K39" s="111"/>
+      <c r="K39" s="110"/>
     </row>
     <row r="40" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A40" s="33">
@@ -8622,7 +8772,7 @@
       <c r="H40" s="62"/>
       <c r="I40" s="61"/>
       <c r="J40" s="62"/>
-      <c r="K40" s="111"/>
+      <c r="K40" s="110"/>
     </row>
     <row r="41" spans="1:17" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A41" s="33">
@@ -8637,7 +8787,7 @@
       <c r="H41" s="62"/>
       <c r="I41" s="61"/>
       <c r="J41" s="62"/>
-      <c r="K41" s="111"/>
+      <c r="K41" s="110"/>
       <c r="M41" s="23"/>
       <c r="N41" s="23"/>
       <c r="O41" s="23"/>
@@ -8657,7 +8807,7 @@
       <c r="H42" s="62"/>
       <c r="I42" s="61"/>
       <c r="J42" s="62"/>
-      <c r="K42" s="111"/>
+      <c r="K42" s="110"/>
       <c r="M42" s="23"/>
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
@@ -8677,7 +8827,7 @@
       <c r="H43" s="62"/>
       <c r="I43" s="61"/>
       <c r="J43" s="62"/>
-      <c r="K43" s="111"/>
+      <c r="K43" s="110"/>
       <c r="M43" s="23"/>
       <c r="N43" s="23"/>
       <c r="O43" s="23"/>
@@ -8697,7 +8847,7 @@
       <c r="H44" s="62"/>
       <c r="I44" s="61"/>
       <c r="J44" s="62"/>
-      <c r="K44" s="111"/>
+      <c r="K44" s="110"/>
       <c r="M44" s="23"/>
       <c r="N44" s="23"/>
       <c r="O44" s="23"/>
@@ -8717,7 +8867,7 @@
       <c r="H45" s="62"/>
       <c r="I45" s="61"/>
       <c r="J45" s="62"/>
-      <c r="K45" s="111"/>
+      <c r="K45" s="110"/>
       <c r="M45" s="23"/>
       <c r="N45" s="23"/>
       <c r="O45" s="23"/>
@@ -8737,7 +8887,7 @@
       <c r="H46" s="62"/>
       <c r="I46" s="61"/>
       <c r="J46" s="62"/>
-      <c r="K46" s="111"/>
+      <c r="K46" s="110"/>
       <c r="M46" s="23"/>
       <c r="N46" s="23"/>
       <c r="O46" s="23"/>
@@ -8757,7 +8907,7 @@
       <c r="H47" s="62"/>
       <c r="I47" s="61"/>
       <c r="J47" s="62"/>
-      <c r="K47" s="111"/>
+      <c r="K47" s="110"/>
       <c r="M47" s="23"/>
       <c r="N47" s="23"/>
       <c r="O47" s="23"/>
@@ -8777,7 +8927,7 @@
       <c r="H48" s="62"/>
       <c r="I48" s="61"/>
       <c r="J48" s="62"/>
-      <c r="K48" s="111"/>
+      <c r="K48" s="110"/>
       <c r="M48" s="23"/>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
@@ -8797,7 +8947,7 @@
       <c r="H49" s="62"/>
       <c r="I49" s="61"/>
       <c r="J49" s="62"/>
-      <c r="K49" s="111"/>
+      <c r="K49" s="110"/>
       <c r="M49" s="23"/>
       <c r="N49" s="23"/>
       <c r="O49" s="23"/>
@@ -8817,7 +8967,7 @@
       <c r="H50" s="62"/>
       <c r="I50" s="61"/>
       <c r="J50" s="62"/>
-      <c r="K50" s="111"/>
+      <c r="K50" s="110"/>
       <c r="M50" s="23"/>
       <c r="N50" s="23"/>
       <c r="O50" s="23"/>
@@ -8837,7 +8987,7 @@
       <c r="H51" s="62"/>
       <c r="I51" s="61"/>
       <c r="J51" s="62"/>
-      <c r="K51" s="111"/>
+      <c r="K51" s="110"/>
       <c r="M51" s="23"/>
       <c r="N51" s="23"/>
       <c r="O51" s="23"/>
@@ -8857,7 +9007,7 @@
       <c r="H52" s="62"/>
       <c r="I52" s="61"/>
       <c r="J52" s="62"/>
-      <c r="K52" s="111"/>
+      <c r="K52" s="110"/>
       <c r="M52" s="23"/>
       <c r="N52" s="23"/>
       <c r="O52" s="23"/>
@@ -8877,7 +9027,7 @@
       <c r="H53" s="62"/>
       <c r="I53" s="61"/>
       <c r="J53" s="62"/>
-      <c r="K53" s="111"/>
+      <c r="K53" s="110"/>
       <c r="M53" s="23"/>
       <c r="N53" s="23"/>
       <c r="O53" s="23"/>
@@ -8897,7 +9047,7 @@
       <c r="H54" s="62"/>
       <c r="I54" s="61"/>
       <c r="J54" s="62"/>
-      <c r="K54" s="111"/>
+      <c r="K54" s="110"/>
       <c r="M54" s="23"/>
       <c r="N54" s="23"/>
       <c r="O54" s="23"/>
@@ -8932,7 +9082,7 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G5"/>
+      <selection activeCell="A6" sqref="A6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -8959,29 +9109,29 @@
       <c r="A1" s="191" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="124"/>
+      <c r="B1" s="123"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="105" t="str">
+      <c r="D1" s="104" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="102" t="str">
+      <c r="F1" s="101" t="str">
         <f>'Update History'!F1</f>
         <v>CRMFXXX4</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="113" t="str">
+      <c r="H1" s="112" t="str">
         <f>'Update History'!H1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="102" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="50"/>
@@ -8990,29 +9140,29 @@
     </row>
     <row r="2" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1">
       <c r="A2" s="192"/>
-      <c r="B2" s="125"/>
+      <c r="B2" s="124"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="105" t="str">
+      <c r="D2" s="104" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - CRM</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="102" t="str">
+      <c r="F2" s="101" t="str">
         <f>'Update History'!F2</f>
         <v>Báo cáo khách hàng không phát sinh đơn hàng</v>
       </c>
-      <c r="G2" s="103" t="s">
+      <c r="G2" s="102" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="51">
         <f>'Update History'!H2</f>
         <v>42401</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="I2" s="102" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="50"/>
@@ -9020,10 +9170,10 @@
       <c r="L2" s="52"/>
     </row>
     <row r="4" spans="1:12" s="23" customFormat="1" ht="11.25">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="121" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="24" t="s">
@@ -9032,7 +9182,7 @@
       <c r="D4" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="100" t="s">
         <v>46</v>
       </c>
       <c r="F4" s="162" t="s">
@@ -9053,7 +9203,7 @@
         <v>161</v>
       </c>
       <c r="C5" s="33"/>
-      <c r="D5" s="131" t="s">
+      <c r="D5" s="130" t="s">
         <v>134</v>
       </c>
       <c r="E5" s="32"/>
@@ -9071,13 +9221,21 @@
       <c r="A6" s="33">
         <v>2</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="33" t="s">
+        <v>161</v>
+      </c>
       <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="D6" s="130" t="s">
+        <v>134</v>
+      </c>
       <c r="E6" s="32"/>
-      <c r="F6" s="189"/>
+      <c r="F6" s="189" t="s">
+        <v>212</v>
+      </c>
       <c r="G6" s="190"/>
-      <c r="H6" s="193"/>
+      <c r="H6" s="193" t="s">
+        <v>213</v>
+      </c>
       <c r="I6" s="194"/>
       <c r="J6" s="195"/>
     </row>
@@ -10084,7 +10242,7 @@
   <dimension ref="A1:T1048467"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="J16" sqref="J16:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -10198,7 +10356,7 @@
       <c r="A4" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="122" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="68" t="s">
@@ -10265,7 +10423,7 @@
       <c r="H5" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="132" t="s">
+      <c r="I5" s="131" t="s">
         <v>184</v>
       </c>
       <c r="J5" s="196" t="s">
@@ -10274,7 +10432,7 @@
       <c r="K5" s="197"/>
       <c r="L5" s="197"/>
       <c r="M5" s="198"/>
-      <c r="N5" s="126" t="s">
+      <c r="N5" s="125" t="s">
         <v>190</v>
       </c>
       <c r="O5" s="89" t="s">
@@ -10311,7 +10469,7 @@
       <c r="H6" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="132" t="s">
+      <c r="I6" s="131" t="s">
         <v>185</v>
       </c>
       <c r="J6" s="196" t="s">
@@ -10320,10 +10478,10 @@
       <c r="K6" s="197"/>
       <c r="L6" s="197"/>
       <c r="M6" s="198"/>
-      <c r="N6" s="126" t="s">
+      <c r="N6" s="125" t="s">
         <v>134</v>
       </c>
-      <c r="O6" s="126" t="s">
+      <c r="O6" s="125" t="s">
         <v>189</v>
       </c>
       <c r="P6" s="76" t="s">
@@ -10342,44 +10500,76 @@
       <c r="A7" s="33">
         <v>3</v>
       </c>
-      <c r="B7" s="33"/>
+      <c r="B7" s="33" t="s">
+        <v>161</v>
+      </c>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="196"/>
+      <c r="F7" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="H7" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="131" t="s">
+        <v>215</v>
+      </c>
+      <c r="J7" s="196" t="s">
+        <v>216</v>
+      </c>
       <c r="K7" s="197"/>
       <c r="L7" s="197"/>
       <c r="M7" s="198"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
+      <c r="N7" s="125" t="s">
+        <v>134</v>
+      </c>
+      <c r="O7" s="125" t="s">
+        <v>191</v>
+      </c>
       <c r="P7" s="76"/>
       <c r="Q7" s="75"/>
       <c r="R7" s="82"/>
       <c r="S7" s="64"/>
       <c r="T7" s="64"/>
     </row>
-    <row r="8" spans="1:20" s="34" customFormat="1" ht="11.25">
+    <row r="8" spans="1:20" s="34" customFormat="1" ht="157.5">
       <c r="A8" s="33">
         <v>4</v>
       </c>
-      <c r="B8" s="33"/>
+      <c r="B8" s="33" t="s">
+        <v>161</v>
+      </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="196"/>
+      <c r="F8" s="132" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="131" t="s">
+        <v>218</v>
+      </c>
+      <c r="J8" s="196" t="s">
+        <v>221</v>
+      </c>
       <c r="K8" s="197"/>
       <c r="L8" s="197"/>
       <c r="M8" s="198"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
+      <c r="N8" s="125" t="s">
+        <v>219</v>
+      </c>
+      <c r="O8" s="125" t="s">
+        <v>220</v>
+      </c>
       <c r="P8" s="76"/>
       <c r="Q8" s="75"/>
       <c r="R8" s="82"/>
@@ -12516,8 +12706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -12753,7 +12943,7 @@
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="B17" s="43"/>
       <c r="C17" s="43" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
@@ -12860,7 +13050,9 @@
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="73"/>
-      <c r="B26" s="43"/>
+      <c r="B26" s="43" t="s">
+        <v>223</v>
+      </c>
       <c r="C26" s="43"/>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
@@ -13141,7 +13333,7 @@
     </row>
     <row r="49" spans="1:10" ht="12" customHeight="1">
       <c r="B49" s="80" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C49" s="86"/>
       <c r="D49" s="43"/>

</xml_diff>